<commit_message>
subo avance en informe y en excel
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaswolff/Desktop/25_20/TECNOLOGIAS_DEL_HORMIGON/TAREAS/TH_TALLER_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaswolff/Desktop/25_20/TECNOLOGIAS_DEL_HORMIGON/TAREAS/TALLER_HA_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8B0D3E-E1A4-3249-ABFD-235B4149BDD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9D201A-63E2-7045-ABCB-0F208C2C003A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{9C17EDB2-E79E-E547-A673-26F1EAF70D3A}"/>
+    <workbookView xWindow="-38400" yWindow="-1020" windowWidth="38400" windowHeight="21600" xr2:uid="{9C17EDB2-E79E-E547-A673-26F1EAF70D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="DESARROLLO" sheetId="2" r:id="rId1"/>
     <sheet name="DATOS" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="79">
   <si>
     <t>GRUPO 1</t>
   </si>
@@ -255,13 +255,55 @@
   <si>
     <t>Cumle f3 mayor a fc + k1</t>
   </si>
+  <si>
+    <t>Prom</t>
+  </si>
+  <si>
+    <t>Numero de aprobados</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Nivel Control Testigos</t>
+  </si>
+  <si>
+    <t>Tabla 1 NCh 1171</t>
+  </si>
+  <si>
+    <t>Esbeltez</t>
+  </si>
+  <si>
+    <t>K1</t>
+  </si>
+  <si>
+    <t>Tabla 2 NCh 1171</t>
+  </si>
+  <si>
+    <t>Resistencia Cilindro</t>
+  </si>
+  <si>
+    <t>K2</t>
+  </si>
+  <si>
+    <t>R cubo</t>
+  </si>
+  <si>
+    <t>R cilindro</t>
+  </si>
+  <si>
+    <t>Rpm</t>
+  </si>
+  <si>
+    <t>Cumple</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -491,7 +533,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -512,7 +554,7 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -528,6 +570,35 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -539,38 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -912,1045 +951,1128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D97EA0-F291-AB40-8238-A1650B046FB5}">
-  <dimension ref="B2:AB62"/>
+  <dimension ref="B2:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="62" workbookViewId="0">
-      <selection activeCell="U38" sqref="U38"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="119" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="16"/>
   <cols>
     <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" customWidth="1"/>
     <col min="7" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="7.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="4.83203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10.5" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="4.5" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="32" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
-      <c r="M2" s="33"/>
-      <c r="N2" s="33"/>
-      <c r="P2" s="34" t="s">
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="P2" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="34"/>
-      <c r="T2" s="34"/>
-      <c r="U2" s="34"/>
-      <c r="V2" s="34"/>
-      <c r="W2" s="34"/>
-      <c r="X2" s="34"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="34"/>
-      <c r="AA2" s="34"/>
-      <c r="AB2" s="34"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+      <c r="Z2" s="29"/>
+      <c r="AA2" s="29"/>
+      <c r="AB2" s="29"/>
     </row>
     <row r="4" spans="2:28">
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C4" s="20">
+      <c r="C4" s="16">
         <v>55</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="37"/>
-      <c r="R4" s="37"/>
-      <c r="S4" s="37"/>
-      <c r="T4" s="37"/>
-      <c r="U4" s="37"/>
-      <c r="W4" s="37" t="s">
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="W4" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="X4" s="37"/>
-      <c r="Y4" s="37"/>
-      <c r="Z4" s="37"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="37"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
     </row>
     <row r="5" spans="2:28">
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="26">
         <v>20</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="P5" s="29" t="s">
+      <c r="P5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="Q5" s="29" t="s">
+      <c r="Q5" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="29" t="s">
+      <c r="R5" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="29" t="s">
+      <c r="S5" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="29" t="s">
+      <c r="T5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="U5" s="29" t="s">
+      <c r="U5" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="W5" s="29" t="s">
+      <c r="W5" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="X5" s="29" t="s">
+      <c r="X5" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="Y5" s="29" t="s">
+      <c r="Y5" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="Z5" s="29" t="s">
+      <c r="Z5" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="AA5" s="29" t="s">
+      <c r="AA5" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="AB5" s="29" t="s">
+      <c r="AB5" s="22" t="s">
         <v>48</v>
       </c>
     </row>
     <row r="6" spans="2:28">
-      <c r="P6" s="18">
+      <c r="P6" s="14">
         <v>5</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="R6" s="18">
+      <c r="R6" s="14">
         <v>0.3</v>
       </c>
-      <c r="S6" s="18">
+      <c r="S6" s="14">
         <v>0.5</v>
       </c>
-      <c r="T6" s="18">
+      <c r="T6" s="14">
         <v>0.8</v>
       </c>
-      <c r="U6" s="18">
+      <c r="U6" s="14">
         <v>1</v>
       </c>
-      <c r="W6" s="18">
+      <c r="W6" s="14">
         <v>5</v>
       </c>
-      <c r="X6" s="18" t="s">
+      <c r="X6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="Y6" s="18">
+      <c r="Y6" s="14">
         <v>0.6</v>
       </c>
-      <c r="Z6" s="18">
+      <c r="Z6" s="14">
         <v>1.2</v>
       </c>
-      <c r="AA6" s="18">
+      <c r="AA6" s="14">
         <v>1.9</v>
       </c>
-      <c r="AB6" s="18">
+      <c r="AB6" s="14">
         <v>2.5</v>
       </c>
     </row>
     <row r="7" spans="2:28">
-      <c r="B7" s="19" t="str">
+      <c r="B7" s="15" t="str">
         <f>DATOS!F98</f>
         <v>Correlativo</v>
       </c>
-      <c r="C7" s="19" t="str">
+      <c r="C7" s="15" t="str">
         <f>DATOS!G98</f>
         <v>7 días [MPa]</v>
       </c>
-      <c r="D7" s="19" t="str">
+      <c r="D7" s="15" t="str">
         <f>DATOS!H98</f>
         <v>28 días [MPa]</v>
       </c>
-      <c r="E7" s="19" t="str">
+      <c r="E7" s="15" t="str">
         <f>DATOS!I98</f>
         <v>28 días [MPa]</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="19" t="str">
+      <c r="G7" s="15" t="str">
         <f>DATOS!K98</f>
         <v>Testigo</v>
       </c>
-      <c r="H7" s="21" t="str">
+      <c r="H7" s="17" t="str">
         <f>DATOS!L98</f>
         <v>D [mm]</v>
       </c>
-      <c r="I7" s="19" t="str">
+      <c r="I7" s="15" t="str">
         <f>DATOS!M98</f>
         <v>H original [mm]</v>
       </c>
-      <c r="J7" s="19" t="str">
+      <c r="J7" s="15" t="str">
         <f>DATOS!N98</f>
         <v>H refrentado [mm]</v>
       </c>
-      <c r="K7" s="19" t="str">
+      <c r="K7" s="15" t="str">
         <f>DATOS!O98</f>
         <v>H rectificado [mm]</v>
       </c>
-      <c r="L7" s="19" t="str">
+      <c r="L7" s="15" t="str">
         <f>DATOS!P98</f>
         <v>R [MPa]</v>
       </c>
-      <c r="M7" s="19" t="str">
+      <c r="M7" s="15" t="str">
         <f>DATOS!Q98</f>
         <v>Edad [dias]</v>
       </c>
-      <c r="P7" s="18">
+      <c r="P7" s="14">
         <v>10</v>
       </c>
-      <c r="Q7" s="18" t="s">
+      <c r="Q7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="R7" s="18">
+      <c r="R7" s="14">
         <v>0</v>
       </c>
-      <c r="S7" s="18">
+      <c r="S7" s="14">
         <v>0</v>
       </c>
-      <c r="T7" s="18">
+      <c r="T7" s="14">
         <v>0</v>
       </c>
-      <c r="U7" s="18">
+      <c r="U7" s="14">
         <v>0</v>
       </c>
-      <c r="W7" s="18">
+      <c r="W7" s="14">
         <v>10</v>
       </c>
-      <c r="X7" s="18" t="s">
+      <c r="X7" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="Y7" s="18">
+      <c r="Y7" s="14">
         <v>0.9</v>
       </c>
-      <c r="Z7" s="18">
+      <c r="Z7" s="14">
         <v>1.7</v>
       </c>
-      <c r="AA7" s="18">
+      <c r="AA7" s="14">
         <v>2.6</v>
       </c>
-      <c r="AB7" s="18">
+      <c r="AB7" s="14">
         <v>3.5</v>
       </c>
     </row>
     <row r="8" spans="2:28">
-      <c r="B8" s="18">
+      <c r="B8" s="14">
         <f>DATOS!F99</f>
         <v>1</v>
       </c>
-      <c r="C8" s="18">
+      <c r="C8" s="14">
         <f>DATOS!G99</f>
         <v>41.45</v>
       </c>
-      <c r="D8" s="18">
+      <c r="D8" s="14">
         <f>DATOS!H99</f>
         <v>52.8</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="14">
         <f>DATOS!I99</f>
         <v>54.6</v>
       </c>
-      <c r="G8" s="23">
+      <c r="G8" s="14">
         <f>DATOS!K99</f>
         <v>1</v>
       </c>
-      <c r="H8" s="24">
+      <c r="H8" s="18">
         <f>DATOS!L99</f>
         <v>150</v>
       </c>
-      <c r="I8" s="23">
+      <c r="I8" s="14">
         <f>DATOS!M99</f>
         <v>187</v>
       </c>
-      <c r="J8" s="23">
+      <c r="J8" s="14">
         <f>DATOS!N99</f>
         <v>192</v>
       </c>
-      <c r="K8" s="23">
+      <c r="K8" s="14">
         <f>DATOS!O99</f>
         <v>182</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="14">
         <f>DATOS!P99</f>
         <v>52.2</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="14">
         <f>DATOS!Q99</f>
         <v>45</v>
       </c>
-      <c r="P8" s="18">
+      <c r="P8" s="14">
         <v>20</v>
       </c>
-      <c r="Q8" s="18" t="s">
+      <c r="Q8" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="18">
+      <c r="R8" s="14">
         <v>-0.4</v>
       </c>
-      <c r="S8" s="18">
+      <c r="S8" s="14">
         <v>-0.7</v>
       </c>
-      <c r="T8" s="18">
+      <c r="T8" s="14">
         <v>-1.1000000000000001</v>
       </c>
-      <c r="U8" s="18">
+      <c r="U8" s="14">
         <v>-1.5</v>
       </c>
-      <c r="W8" s="18">
+      <c r="W8" s="14">
         <v>20</v>
       </c>
-      <c r="X8" s="18" t="s">
+      <c r="X8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="Y8" s="18">
+      <c r="Y8" s="14">
         <v>1.4</v>
       </c>
-      <c r="Z8" s="18">
+      <c r="Z8" s="14">
         <v>2.7</v>
       </c>
-      <c r="AA8" s="18">
+      <c r="AA8" s="14">
         <v>4.0999999999999996</v>
       </c>
-      <c r="AB8" s="18">
+      <c r="AB8" s="14">
         <v>5.5</v>
       </c>
     </row>
     <row r="9" spans="2:28">
-      <c r="B9" s="18">
+      <c r="B9" s="14">
         <f>DATOS!F100</f>
         <v>2</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="14">
         <f>DATOS!G100</f>
         <v>40.200000000000003</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="14">
         <f>DATOS!H100</f>
         <v>57.11</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="14">
         <f>DATOS!I100</f>
         <v>56.6</v>
       </c>
-      <c r="G9" s="23">
+      <c r="G9" s="14">
         <f>DATOS!K100</f>
         <v>2</v>
       </c>
-      <c r="H9" s="24">
+      <c r="H9" s="18">
         <f>DATOS!L100</f>
         <v>150</v>
       </c>
-      <c r="I9" s="23">
+      <c r="I9" s="14">
         <f>DATOS!M100</f>
         <v>190</v>
       </c>
-      <c r="J9" s="23">
+      <c r="J9" s="14">
         <f>DATOS!N100</f>
         <v>195</v>
       </c>
-      <c r="K9" s="23">
+      <c r="K9" s="14">
         <f>DATOS!O100</f>
         <v>185</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="14">
         <f>DATOS!P100</f>
         <v>53.5</v>
       </c>
-      <c r="M9" s="23">
+      <c r="M9" s="14">
         <f>DATOS!Q100</f>
         <v>45</v>
       </c>
     </row>
     <row r="10" spans="2:28">
-      <c r="B10" s="18">
+      <c r="B10" s="14">
         <f>DATOS!F101</f>
         <v>3</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="14">
         <f>DATOS!G101</f>
         <v>43.5</v>
       </c>
-      <c r="D10" s="18">
+      <c r="D10" s="14">
         <f>DATOS!H101</f>
         <v>52.35</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="14">
         <f>DATOS!I101</f>
         <v>55.18</v>
       </c>
-      <c r="G10" s="26">
+      <c r="G10" s="20">
         <f>DATOS!K101</f>
         <v>3</v>
       </c>
-      <c r="H10" s="27">
+      <c r="H10" s="21">
         <f>DATOS!L101</f>
         <v>150</v>
       </c>
-      <c r="I10" s="26">
+      <c r="I10" s="20">
         <f>DATOS!M101</f>
         <v>185</v>
       </c>
-      <c r="J10" s="26">
+      <c r="J10" s="20">
         <f>DATOS!N101</f>
         <v>190</v>
       </c>
-      <c r="K10" s="26">
+      <c r="K10" s="20">
         <f>DATOS!O101</f>
         <v>180</v>
       </c>
-      <c r="L10" s="26">
+      <c r="L10" s="20">
         <f>DATOS!P101</f>
         <v>51.5</v>
       </c>
-      <c r="M10" s="26">
+      <c r="M10" s="20">
         <f>DATOS!Q101</f>
         <v>45</v>
       </c>
-      <c r="P10" s="37" t="s">
+      <c r="P10" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="37"/>
-      <c r="R10" s="37"/>
-      <c r="S10" s="37"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="30"/>
+      <c r="S10" s="30"/>
+      <c r="V10" s="30" t="s">
+        <v>69</v>
+      </c>
+      <c r="W10" s="30"/>
     </row>
     <row r="11" spans="2:28">
-      <c r="B11" s="18">
+      <c r="B11" s="14">
         <f>DATOS!F102</f>
         <v>4</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="14">
         <f>DATOS!G102</f>
         <v>41</v>
       </c>
-      <c r="D11" s="18">
+      <c r="D11" s="14">
         <f>DATOS!H102</f>
         <v>55.25</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="14">
         <f>DATOS!I102</f>
         <v>54.2</v>
       </c>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="34" t="s">
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+      <c r="I11" s="19"/>
+      <c r="J11" s="19"/>
+      <c r="K11" s="19"/>
+      <c r="L11" s="19"/>
+      <c r="M11" s="19"/>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="34"/>
-      <c r="S11" s="34"/>
+      <c r="R11" s="29"/>
+      <c r="S11" s="29"/>
+      <c r="V11" s="22" t="s">
+        <v>70</v>
+      </c>
+      <c r="W11" s="22" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="12" spans="2:28">
-      <c r="B12" s="18">
+      <c r="B12" s="14">
         <f>DATOS!F103</f>
         <v>5</v>
       </c>
-      <c r="C12" s="18">
+      <c r="C12" s="14">
         <f>DATOS!G103</f>
         <v>40</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="14">
         <f>DATOS!H103</f>
         <v>54.48</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="14">
         <f>DATOS!I103</f>
         <v>53.82</v>
       </c>
-      <c r="G12" s="22"/>
-      <c r="H12" s="22"/>
-      <c r="I12" s="22"/>
-      <c r="J12" s="22"/>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="22"/>
-      <c r="P12" s="29" t="s">
+      <c r="P12" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="Q12" s="18">
+      <c r="Q12" s="14">
         <v>5</v>
       </c>
-      <c r="R12" s="18">
+      <c r="R12" s="14">
         <v>10</v>
       </c>
-      <c r="S12" s="18">
+      <c r="S12" s="14">
         <v>20</v>
       </c>
+      <c r="V12" s="14">
+        <v>2</v>
+      </c>
+      <c r="W12" s="14">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="2:28">
-      <c r="B13" s="18">
+      <c r="B13" s="14">
         <f>DATOS!F104</f>
         <v>6</v>
       </c>
-      <c r="C13" s="18">
+      <c r="C13" s="14">
         <f>DATOS!G104</f>
         <v>41</v>
       </c>
-      <c r="D13" s="18">
+      <c r="D13" s="14">
         <f>DATOS!H104</f>
         <v>55.3</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="14">
         <f>DATOS!I104</f>
         <v>52.08</v>
       </c>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="22"/>
-      <c r="J13" s="22"/>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="22"/>
-      <c r="P13" s="18">
+      <c r="P13" s="14">
         <v>3</v>
       </c>
-      <c r="Q13" s="18">
+      <c r="Q13" s="14">
         <v>2.92</v>
       </c>
-      <c r="R13" s="18">
+      <c r="R13" s="14">
         <v>1.8859999999999999</v>
       </c>
-      <c r="S13" s="18">
+      <c r="S13" s="14">
         <v>1.0609999999999999</v>
       </c>
+      <c r="V13" s="14">
+        <v>1.75</v>
+      </c>
+      <c r="W13" s="14">
+        <v>0.98</v>
+      </c>
     </row>
     <row r="14" spans="2:28">
-      <c r="B14" s="18">
+      <c r="B14" s="14">
         <f>DATOS!F105</f>
         <v>7</v>
       </c>
-      <c r="C14" s="18">
+      <c r="C14" s="14">
         <f>DATOS!G105</f>
         <v>43.5</v>
       </c>
-      <c r="D14" s="18">
+      <c r="D14" s="14">
         <f>DATOS!H105</f>
         <v>51</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="14">
         <f>DATOS!I105</f>
         <v>53.82</v>
       </c>
-      <c r="P14" s="18">
+      <c r="P14" s="14">
         <v>4</v>
       </c>
-      <c r="Q14" s="18">
+      <c r="Q14" s="14">
         <v>2.3530000000000002</v>
       </c>
-      <c r="R14" s="18">
+      <c r="R14" s="14">
         <v>1.6379999999999999</v>
       </c>
-      <c r="S14" s="18">
+      <c r="S14" s="14">
         <v>0.97799999999999998</v>
       </c>
+      <c r="V14" s="14">
+        <v>1.5</v>
+      </c>
+      <c r="W14" s="14">
+        <v>0.96</v>
+      </c>
     </row>
     <row r="15" spans="2:28">
-      <c r="B15" s="18">
+      <c r="B15" s="14">
         <f>DATOS!F106</f>
         <v>8</v>
       </c>
-      <c r="C15" s="18">
+      <c r="C15" s="14">
         <f>DATOS!G106</f>
         <v>41</v>
       </c>
-      <c r="D15" s="18">
+      <c r="D15" s="14">
         <f>DATOS!H106</f>
         <v>48.4</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="14">
         <f>DATOS!I106</f>
         <v>49.9</v>
       </c>
-      <c r="P15" s="18">
+      <c r="P15" s="14">
         <v>5</v>
       </c>
-      <c r="Q15" s="18">
+      <c r="Q15" s="14">
         <v>2.1320000000000001</v>
       </c>
-      <c r="R15" s="18">
+      <c r="R15" s="14">
         <v>1.5329999999999999</v>
       </c>
-      <c r="S15" s="18">
+      <c r="S15" s="14">
         <v>0.94099999999999995</v>
       </c>
+      <c r="V15" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="W15" s="14">
+        <v>0.93</v>
+      </c>
     </row>
     <row r="16" spans="2:28">
-      <c r="B16" s="18">
+      <c r="B16" s="14">
         <f>DATOS!F107</f>
         <v>9</v>
       </c>
-      <c r="C16" s="18">
+      <c r="C16" s="14">
         <f>DATOS!G107</f>
         <v>40</v>
       </c>
-      <c r="D16" s="18">
+      <c r="D16" s="14">
         <f>DATOS!H107</f>
         <v>49.5</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="14">
         <f>DATOS!I107</f>
         <v>45.6</v>
       </c>
-      <c r="P16" s="18">
+      <c r="P16" s="14">
         <v>6</v>
       </c>
-      <c r="Q16" s="18">
+      <c r="Q16" s="14">
         <v>2.0150000000000001</v>
       </c>
-      <c r="R16" s="18">
+      <c r="R16" s="14">
         <v>1.476</v>
       </c>
-      <c r="S16" s="18">
+      <c r="S16" s="14">
         <v>0.92</v>
       </c>
-    </row>
-    <row r="17" spans="2:19">
-      <c r="B17" s="18">
+      <c r="V16" s="14">
+        <v>1</v>
+      </c>
+      <c r="W16" s="14">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="17" spans="2:29">
+      <c r="B17" s="14">
         <f>DATOS!F108</f>
         <v>10</v>
       </c>
-      <c r="C17" s="18">
+      <c r="C17" s="14">
         <f>DATOS!G108</f>
         <v>40.200000000000003</v>
       </c>
-      <c r="D17" s="18">
+      <c r="D17" s="14">
         <f>DATOS!H108</f>
         <v>52.56</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="14">
         <f>DATOS!I108</f>
         <v>47.88</v>
       </c>
-      <c r="P17" s="18">
+      <c r="P17" s="14">
         <v>7</v>
       </c>
-      <c r="Q17" s="18">
+      <c r="Q17" s="14">
         <v>1.9430000000000001</v>
       </c>
-      <c r="R17" s="18">
+      <c r="R17" s="14">
         <v>1.44</v>
       </c>
-      <c r="S17" s="18">
+      <c r="S17" s="14">
         <v>0.90600000000000003</v>
       </c>
     </row>
-    <row r="18" spans="2:19">
-      <c r="B18" s="18">
+    <row r="18" spans="2:29">
+      <c r="B18" s="14">
         <f>DATOS!F109</f>
         <v>11</v>
       </c>
-      <c r="C18" s="18">
+      <c r="C18" s="14">
         <f>DATOS!G109</f>
         <v>43.5</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="14">
         <f>DATOS!H109</f>
         <v>57.11</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="14">
         <f>DATOS!I109</f>
         <v>56.6</v>
       </c>
-      <c r="P18" s="18">
+      <c r="P18" s="14">
         <v>8</v>
       </c>
-      <c r="Q18" s="18">
+      <c r="Q18" s="14">
         <v>1.895</v>
       </c>
-      <c r="R18" s="18">
+      <c r="R18" s="14">
         <v>1.415</v>
       </c>
-      <c r="S18" s="18">
+      <c r="S18" s="14">
         <v>0.89600000000000002</v>
       </c>
-    </row>
-    <row r="19" spans="2:19">
-      <c r="B19" s="18">
+      <c r="V18" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="W18" s="30"/>
+      <c r="X18" s="30"/>
+      <c r="Y18" s="30"/>
+      <c r="Z18" s="30"/>
+      <c r="AA18" s="30"/>
+      <c r="AB18" s="30"/>
+      <c r="AC18" s="30"/>
+    </row>
+    <row r="19" spans="2:29">
+      <c r="B19" s="14">
         <f>DATOS!F110</f>
         <v>12</v>
       </c>
-      <c r="C19" s="18">
+      <c r="C19" s="14">
         <f>DATOS!G110</f>
         <v>40</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="14">
         <f>DATOS!H110</f>
         <v>52.35</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="14">
         <f>DATOS!I110</f>
         <v>52.08</v>
       </c>
-      <c r="P19" s="18">
+      <c r="P19" s="14">
         <v>9</v>
       </c>
-      <c r="Q19" s="18">
+      <c r="Q19" s="14">
         <v>1.86</v>
       </c>
-      <c r="R19" s="18">
+      <c r="R19" s="14">
         <v>1.397</v>
       </c>
-      <c r="S19" s="18">
+      <c r="S19" s="14">
         <v>0.88900000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="2:19">
-      <c r="B20" s="18">
+      <c r="V19" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="W19" s="14">
+        <v>20</v>
+      </c>
+      <c r="X19" s="14">
+        <v>25</v>
+      </c>
+      <c r="Y19" s="14">
+        <v>30</v>
+      </c>
+      <c r="Z19" s="14">
+        <v>35</v>
+      </c>
+      <c r="AA19" s="14">
+        <v>40</v>
+      </c>
+      <c r="AB19" s="14">
+        <v>45</v>
+      </c>
+      <c r="AC19" s="14">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="2:29">
+      <c r="B20" s="14">
         <f>DATOS!F111</f>
         <v>13</v>
       </c>
-      <c r="C20" s="18">
+      <c r="C20" s="14">
         <f>DATOS!G111</f>
         <v>41</v>
       </c>
-      <c r="D20" s="18">
+      <c r="D20" s="14">
         <f>DATOS!H111</f>
         <v>55.25</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="14">
         <f>DATOS!I111</f>
         <v>53.82</v>
       </c>
-      <c r="P20" s="18">
+      <c r="P20" s="14">
         <v>10</v>
       </c>
-      <c r="Q20" s="18">
+      <c r="Q20" s="14">
         <v>1.833</v>
       </c>
-      <c r="R20" s="18">
+      <c r="R20" s="14">
         <v>1.383</v>
       </c>
-      <c r="S20" s="18">
+      <c r="S20" s="14">
         <v>0.88300000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="2:19">
-      <c r="B21" s="18">
+      <c r="V20" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="W20" s="14">
+        <v>1.25</v>
+      </c>
+      <c r="X20" s="14">
+        <v>1.2</v>
+      </c>
+      <c r="Y20" s="14">
+        <v>1.17</v>
+      </c>
+      <c r="Z20" s="14">
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="AA20" s="14">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="AB20" s="14">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="AC20" s="14">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="2:29">
+      <c r="B21" s="14">
         <f>DATOS!F112</f>
         <v>14</v>
       </c>
-      <c r="C21" s="18">
+      <c r="C21" s="14">
         <f>DATOS!G112</f>
         <v>43.5</v>
       </c>
-      <c r="D21" s="18">
+      <c r="D21" s="14">
         <f>DATOS!H112</f>
         <v>54.48</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="14">
         <f>DATOS!I112</f>
         <v>53.82</v>
       </c>
-      <c r="P21" s="18">
+      <c r="P21" s="14">
         <v>11</v>
       </c>
-      <c r="Q21" s="18">
+      <c r="Q21" s="14">
         <v>1.8120000000000001</v>
       </c>
-      <c r="R21" s="18">
+      <c r="R21" s="14">
         <v>1.3720000000000001</v>
       </c>
-      <c r="S21" s="18">
+      <c r="S21" s="14">
         <v>0.879</v>
       </c>
     </row>
-    <row r="22" spans="2:19">
-      <c r="B22" s="18">
+    <row r="22" spans="2:29">
+      <c r="B22" s="14">
         <f>DATOS!F113</f>
         <v>15</v>
       </c>
-      <c r="C22" s="18">
+      <c r="C22" s="14">
         <f>DATOS!G113</f>
         <v>41</v>
       </c>
-      <c r="D22" s="18">
+      <c r="D22" s="14">
         <f>DATOS!H113</f>
         <v>55.3</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="14">
         <f>DATOS!I113</f>
         <v>57.79</v>
       </c>
-      <c r="P22" s="18">
+      <c r="P22" s="14">
         <v>12</v>
       </c>
-      <c r="Q22" s="18">
+      <c r="Q22" s="14">
         <v>1.796</v>
       </c>
-      <c r="R22" s="18">
+      <c r="R22" s="14">
         <v>1.363</v>
       </c>
-      <c r="S22" s="18">
+      <c r="S22" s="14">
         <v>0.876</v>
       </c>
     </row>
-    <row r="23" spans="2:19">
-      <c r="B23" s="18">
+    <row r="23" spans="2:29">
+      <c r="B23" s="14">
         <f>DATOS!F114</f>
         <v>16</v>
       </c>
-      <c r="C23" s="18">
+      <c r="C23" s="14">
         <f>DATOS!G114</f>
         <v>40</v>
       </c>
-      <c r="D23" s="18">
+      <c r="D23" s="14">
         <f>DATOS!H114</f>
         <v>58.15</v>
       </c>
-      <c r="E23" s="18">
+      <c r="E23" s="14">
         <f>DATOS!I114</f>
         <v>56.6</v>
       </c>
-      <c r="P23" s="18">
+      <c r="P23" s="14">
         <v>13</v>
       </c>
-      <c r="Q23" s="18">
+      <c r="Q23" s="14">
         <v>1.782</v>
       </c>
-      <c r="R23" s="18">
+      <c r="R23" s="14">
         <v>1.3560000000000001</v>
       </c>
-      <c r="S23" s="18">
+      <c r="S23" s="14">
         <v>0.873</v>
       </c>
     </row>
-    <row r="24" spans="2:19">
-      <c r="B24" s="18">
+    <row r="24" spans="2:29">
+      <c r="B24" s="14">
         <f>DATOS!F115</f>
         <v>17</v>
       </c>
-      <c r="C24" s="18">
+      <c r="C24" s="14">
         <f>DATOS!G115</f>
         <v>40.200000000000003</v>
       </c>
-      <c r="D24" s="18">
+      <c r="D24" s="14">
         <f>DATOS!H115</f>
         <v>55.25</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="14">
         <f>DATOS!I115</f>
         <v>55.18</v>
       </c>
-      <c r="P24" s="18">
+      <c r="P24" s="14">
         <v>14</v>
       </c>
-      <c r="Q24" s="18">
+      <c r="Q24" s="14">
         <v>1.7709999999999999</v>
       </c>
-      <c r="R24" s="18">
+      <c r="R24" s="14">
         <v>1.35</v>
       </c>
-      <c r="S24" s="18">
+      <c r="S24" s="14">
         <v>0.87</v>
       </c>
     </row>
-    <row r="25" spans="2:19">
-      <c r="B25" s="18">
+    <row r="25" spans="2:29">
+      <c r="B25" s="14">
         <f>DATOS!F116</f>
         <v>18</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="14">
         <f>DATOS!G116</f>
         <v>43.5</v>
       </c>
-      <c r="D25" s="18">
+      <c r="D25" s="14">
         <f>DATOS!H116</f>
         <v>52.56</v>
       </c>
-      <c r="E25" s="18">
+      <c r="E25" s="14">
         <f>DATOS!I116</f>
         <v>53.82</v>
       </c>
-      <c r="P25" s="18">
+      <c r="P25" s="14">
         <v>15</v>
       </c>
-      <c r="Q25" s="18">
+      <c r="Q25" s="14">
         <v>1.7609999999999999</v>
       </c>
-      <c r="R25" s="18">
+      <c r="R25" s="14">
         <v>1.345</v>
       </c>
-      <c r="S25" s="18">
+      <c r="S25" s="14">
         <v>0.86799999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:19">
-      <c r="B26" s="18">
+    <row r="26" spans="2:29">
+      <c r="B26" s="14">
         <f>DATOS!F117</f>
         <v>19</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="14">
         <f>DATOS!G117</f>
         <v>41</v>
       </c>
-      <c r="D26" s="18">
+      <c r="D26" s="14">
         <f>DATOS!H117</f>
         <v>48.4</v>
       </c>
-      <c r="E26" s="18">
+      <c r="E26" s="14">
         <f>DATOS!I117</f>
         <v>45.68</v>
       </c>
-      <c r="P26" s="18">
+      <c r="P26" s="14">
         <v>16</v>
       </c>
-      <c r="Q26" s="18">
+      <c r="Q26" s="14">
         <v>1.7529999999999999</v>
       </c>
-      <c r="R26" s="18">
+      <c r="R26" s="14">
         <v>1.341</v>
       </c>
-      <c r="S26" s="18">
+      <c r="S26" s="14">
         <v>0.86599999999999999</v>
       </c>
     </row>
-    <row r="27" spans="2:19">
-      <c r="B27" s="18">
+    <row r="27" spans="2:29">
+      <c r="B27" s="14">
         <f>DATOS!F118</f>
         <v>20</v>
       </c>
-      <c r="C27" s="18">
+      <c r="C27" s="14">
         <f>DATOS!G118</f>
         <v>40</v>
       </c>
-      <c r="D27" s="18">
+      <c r="D27" s="14">
         <f>DATOS!H118</f>
         <v>49.6</v>
       </c>
-      <c r="E27" s="18">
+      <c r="E27" s="14">
         <f>DATOS!I118</f>
         <v>47.7</v>
       </c>
-      <c r="P27" s="18">
+      <c r="P27" s="14">
         <v>17</v>
       </c>
-      <c r="Q27" s="18">
+      <c r="Q27" s="14">
         <v>1.746</v>
       </c>
-      <c r="R27" s="18">
+      <c r="R27" s="14">
         <v>1.337</v>
       </c>
-      <c r="S27" s="18">
+      <c r="S27" s="14">
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="28" spans="2:19">
-      <c r="P28" s="18">
+    <row r="28" spans="2:29">
+      <c r="P28" s="14">
         <v>18</v>
       </c>
-      <c r="Q28" s="18">
+      <c r="Q28" s="14">
         <v>1.74</v>
       </c>
-      <c r="R28" s="18">
+      <c r="R28" s="14">
         <v>1.333</v>
       </c>
-      <c r="S28" s="18">
+      <c r="S28" s="14">
         <v>0.86299999999999999</v>
       </c>
     </row>
-    <row r="29" spans="2:19">
-      <c r="B29" s="28" t="s">
+    <row r="29" spans="2:29">
+      <c r="B29" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="28"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="28"/>
-      <c r="H29" s="28"/>
-      <c r="I29" s="28"/>
-      <c r="J29" s="28"/>
-      <c r="K29" s="28"/>
-      <c r="L29" s="28"/>
-      <c r="M29" s="28"/>
-      <c r="N29" s="28"/>
-      <c r="P29" s="18">
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
+      <c r="H29" s="31"/>
+      <c r="I29" s="31"/>
+      <c r="J29" s="31"/>
+      <c r="K29" s="31"/>
+      <c r="L29" s="31"/>
+      <c r="M29" s="31"/>
+      <c r="N29" s="31"/>
+      <c r="P29" s="14">
         <v>19</v>
       </c>
-      <c r="Q29" s="18">
+      <c r="Q29" s="14">
         <v>1.734</v>
       </c>
-      <c r="R29" s="18">
+      <c r="R29" s="14">
         <v>1.33</v>
       </c>
-      <c r="S29" s="18">
+      <c r="S29" s="14">
         <v>0.86199999999999999</v>
       </c>
     </row>
-    <row r="30" spans="2:19">
-      <c r="P30" s="18">
+    <row r="30" spans="2:29">
+      <c r="P30" s="14">
         <v>20</v>
       </c>
-      <c r="Q30" s="18">
+      <c r="Q30" s="14">
         <v>1.7290000000000001</v>
       </c>
-      <c r="R30" s="18">
+      <c r="R30" s="14">
         <v>1.3280000000000001</v>
       </c>
-      <c r="S30" s="18">
+      <c r="S30" s="14">
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="31" spans="2:19">
-      <c r="B31" s="32" t="s">
+    <row r="31" spans="2:29">
+      <c r="B31" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="C31" s="32" t="s">
+      <c r="C31" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="D31" s="32" t="s">
+      <c r="D31" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="E31" s="32" t="s">
+      <c r="E31" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="H31" s="32" t="s">
+      <c r="H31" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="I31" s="18" cm="1">
+      <c r="I31" s="14" cm="1">
         <f t="array" ref="I31">IF($C$4&lt;=5,
    INDEX($R$5:$R$8,MATCH($C$5,$P$5:$P$8,0)),
    IF($C$4&gt;=20,
@@ -1964,49 +2086,49 @@
 )</f>
         <v>-1.5</v>
       </c>
-      <c r="K31" s="37" t="s">
+      <c r="K31" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="L31" s="37"/>
-      <c r="M31" s="37"/>
-      <c r="P31" s="18">
+      <c r="L31" s="30"/>
+      <c r="M31" s="30"/>
+      <c r="P31" s="14">
         <v>21</v>
       </c>
-      <c r="Q31" s="18">
+      <c r="Q31" s="14">
         <v>1.7250000000000001</v>
       </c>
-      <c r="R31" s="18">
+      <c r="R31" s="14">
         <v>1.325</v>
       </c>
-      <c r="S31" s="18">
+      <c r="S31" s="14">
         <v>0.86</v>
       </c>
     </row>
-    <row r="32" spans="2:19">
-      <c r="B32" s="18">
+    <row r="32" spans="2:29">
+      <c r="B32" s="14">
         <f>B8</f>
         <v>1</v>
       </c>
-      <c r="C32" s="18">
+      <c r="C32" s="14">
         <f>AVERAGE(D8:E8)</f>
         <v>53.7</v>
       </c>
-      <c r="D32" s="18">
+      <c r="D32" s="14">
         <f>($C$52-C32)^2</f>
         <v>0.36090056250000602</v>
       </c>
-      <c r="E32" s="18">
+      <c r="E32" s="14">
         <f>AVERAGE(C32:C34)</f>
         <v>54.773333333333333</v>
       </c>
-      <c r="F32" s="18">
-        <f>ABS(D8-E8)</f>
+      <c r="F32" s="14">
+        <f t="shared" ref="F32:F51" si="0">ABS(D8-E8)</f>
         <v>1.8000000000000043</v>
       </c>
-      <c r="H32" s="32" t="s">
+      <c r="H32" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="18" cm="1">
+      <c r="I32" s="14" cm="1">
         <f t="array" ref="I32">IF($C$4&lt;=5,
    INDEX($Y$5:$Y$8,MATCH($C$5,$W$5:$W$8,0)),
    IF($C$4&gt;=20,
@@ -2019,861 +2141,1064 @@
 )</f>
         <v>5.5</v>
       </c>
-      <c r="K32" s="32" t="s">
+      <c r="K32" s="24" t="s">
         <v>52</v>
       </c>
-      <c r="L32" s="32" t="s">
+      <c r="L32" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="M32" s="32" t="s">
+      <c r="M32" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="P32" s="18">
+      <c r="P32" s="14">
         <v>22</v>
       </c>
-      <c r="Q32" s="18">
+      <c r="Q32" s="14">
         <v>1.7210000000000001</v>
       </c>
-      <c r="R32" s="18">
+      <c r="R32" s="14">
         <v>1.323</v>
       </c>
-      <c r="S32" s="18">
+      <c r="S32" s="14">
         <v>0.85899999999999999</v>
       </c>
     </row>
     <row r="33" spans="2:19">
-      <c r="B33" s="18">
-        <f t="shared" ref="B33:B50" si="0">B9</f>
+      <c r="B33" s="14">
+        <f t="shared" ref="B33:B50" si="1">B9</f>
         <v>2</v>
       </c>
-      <c r="C33" s="18">
-        <f t="shared" ref="C33:C51" si="1">AVERAGE(D9:E9)</f>
+      <c r="C33" s="14">
+        <f t="shared" ref="C33:C51" si="2">AVERAGE(D9:E9)</f>
         <v>56.855000000000004</v>
       </c>
-      <c r="D33" s="18">
-        <f t="shared" ref="D33:D51" si="2">($C$52-C33)^2</f>
+      <c r="D33" s="14">
+        <f t="shared" ref="D33:D51" si="3">($C$52-C33)^2</f>
         <v>14.105658062500046</v>
       </c>
-      <c r="E33" s="18">
-        <f t="shared" ref="E33:E49" si="3">AVERAGE(C33:C35)</f>
+      <c r="E33" s="14">
+        <f t="shared" ref="E33:E49" si="4">AVERAGE(C33:C35)</f>
         <v>55.115000000000002</v>
       </c>
-      <c r="F33" s="18">
-        <f>ABS(D9-E9)</f>
+      <c r="F33" s="14">
+        <f t="shared" si="0"/>
         <v>0.50999999999999801</v>
       </c>
-      <c r="H33" s="32" t="s">
+      <c r="H33" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="I33" s="18">
+      <c r="I33" s="14">
         <f>INDEX($Q$12:$S$40,MATCH(MIN($B$27,30),$P$12:$P$40,0),MATCH($C$5,{5,10,20},0))</f>
         <v>0.86099999999999999</v>
       </c>
-      <c r="K33" s="18">
-        <f>B32</f>
+      <c r="K33" s="14">
+        <f t="shared" ref="K33:K52" si="5">B32</f>
         <v>1</v>
       </c>
-      <c r="L33" s="18">
-        <f>IF(C32 &gt;= $C$4 - $I$32,1,0)</f>
+      <c r="L33" s="14">
+        <f t="shared" ref="L33:L52" si="6">IF(C32 &gt;= $C$4 - $I$32,1,0)</f>
         <v>1</v>
       </c>
-      <c r="M33" s="18">
+      <c r="M33" s="14">
         <f>IF(E32&gt;=$C$4+$I$31,1,0)</f>
         <v>1</v>
       </c>
-      <c r="P33" s="18">
+      <c r="P33" s="14">
         <v>23</v>
       </c>
-      <c r="Q33" s="18">
+      <c r="Q33" s="14">
         <v>1.7170000000000001</v>
       </c>
-      <c r="R33" s="18">
+      <c r="R33" s="14">
         <v>1.321</v>
       </c>
-      <c r="S33" s="18">
+      <c r="S33" s="14">
         <v>0.85799999999999998</v>
       </c>
     </row>
     <row r="34" spans="2:19">
-      <c r="B34" s="18">
+      <c r="B34" s="14">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="C34" s="14">
+        <f t="shared" si="2"/>
+        <v>53.765000000000001</v>
+      </c>
+      <c r="D34" s="14">
+        <f t="shared" si="3"/>
+        <v>0.44322306250000365</v>
+      </c>
+      <c r="E34" s="14">
+        <f t="shared" si="4"/>
+        <v>54.213333333333338</v>
+      </c>
+      <c r="F34" s="14">
         <f t="shared" si="0"/>
+        <v>2.8299999999999983</v>
+      </c>
+      <c r="K34" s="14">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="L34" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M34" s="14">
+        <f t="shared" ref="M34:M50" si="7">IF(E33&gt;=$C$4+$I$31,1,0)</f>
+        <v>1</v>
+      </c>
+      <c r="P34" s="14">
+        <v>24</v>
+      </c>
+      <c r="Q34" s="14">
+        <v>1.714</v>
+      </c>
+      <c r="R34" s="14">
+        <v>1.319</v>
+      </c>
+      <c r="S34" s="14">
+        <v>0.85799999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="2:19">
+      <c r="B35" s="14">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C35" s="14">
+        <f t="shared" si="2"/>
+        <v>54.725000000000001</v>
+      </c>
+      <c r="D35" s="14">
+        <f t="shared" si="3"/>
+        <v>2.6430630625000116</v>
+      </c>
+      <c r="E35" s="14">
+        <f t="shared" si="4"/>
+        <v>54.188333333333333</v>
+      </c>
+      <c r="F35" s="14">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999972</v>
+      </c>
+      <c r="K35" s="14">
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="C34" s="18">
+      <c r="L35" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M35" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="P35" s="14">
+        <v>25</v>
+      </c>
+      <c r="Q35" s="14">
+        <v>1.7110000000000001</v>
+      </c>
+      <c r="R35" s="14">
+        <v>1.3180000000000001</v>
+      </c>
+      <c r="S35" s="14">
+        <v>0.85699999999999998</v>
+      </c>
+    </row>
+    <row r="36" spans="2:19">
+      <c r="B36" s="14">
         <f t="shared" si="1"/>
-        <v>53.765000000000001</v>
-      </c>
-      <c r="D34" s="18">
+        <v>5</v>
+      </c>
+      <c r="C36" s="14">
         <f t="shared" si="2"/>
-        <v>0.44322306250000365</v>
-      </c>
-      <c r="E34" s="18">
+        <v>54.15</v>
+      </c>
+      <c r="D36" s="14">
         <f t="shared" si="3"/>
-        <v>54.213333333333338</v>
-      </c>
-      <c r="F34" s="18">
-        <f>ABS(D10-E10)</f>
-        <v>2.8299999999999983</v>
-      </c>
-      <c r="K34" s="18">
-        <f>B33</f>
-        <v>2</v>
-      </c>
-      <c r="L34" s="18">
-        <f>IF(C33 &gt;= $C$4 - $I$32,1,0)</f>
+        <v>1.1040755625000016</v>
+      </c>
+      <c r="E36" s="14">
+        <f t="shared" si="4"/>
+        <v>53.416666666666664</v>
+      </c>
+      <c r="F36" s="14">
+        <f t="shared" si="0"/>
+        <v>0.65999999999999659</v>
+      </c>
+      <c r="K36" s="14">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="L36" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M34" s="18">
-        <f t="shared" ref="M34:M52" si="4">IF(E33&gt;=$C$4+$I$31,1,0)</f>
+      <c r="M36" s="14">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P34" s="18">
-        <v>24</v>
-      </c>
-      <c r="Q34" s="18">
-        <v>1.714</v>
-      </c>
-      <c r="R34" s="18">
-        <v>1.319</v>
-      </c>
-      <c r="S34" s="18">
-        <v>0.85799999999999998</v>
-      </c>
-    </row>
-    <row r="35" spans="2:19">
-      <c r="B35" s="18">
+      <c r="P36" s="14">
+        <v>26</v>
+      </c>
+      <c r="Q36" s="14">
+        <v>1.708</v>
+      </c>
+      <c r="R36" s="14">
+        <v>1.3160000000000001</v>
+      </c>
+      <c r="S36" s="14">
+        <v>0.85599999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="2:19">
+      <c r="B37" s="14">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C37" s="14">
+        <f t="shared" si="2"/>
+        <v>53.69</v>
+      </c>
+      <c r="D37" s="14">
+        <f t="shared" si="3"/>
+        <v>0.34898556249999985</v>
+      </c>
+      <c r="E37" s="14">
+        <f t="shared" si="4"/>
+        <v>51.75</v>
+      </c>
+      <c r="F37" s="14">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="C35" s="18">
+        <v>3.2199999999999989</v>
+      </c>
+      <c r="K37" s="14">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="L37" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M37" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="14">
+        <v>27</v>
+      </c>
+      <c r="Q37" s="14">
+        <v>1.706</v>
+      </c>
+      <c r="R37" s="14">
+        <v>1.3149999999999999</v>
+      </c>
+      <c r="S37" s="14">
+        <v>0.85599999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="2:19">
+      <c r="B38" s="14">
         <f t="shared" si="1"/>
-        <v>54.725000000000001</v>
-      </c>
-      <c r="D35" s="18">
+        <v>7</v>
+      </c>
+      <c r="C38" s="14">
         <f t="shared" si="2"/>
-        <v>2.6430630625000116</v>
-      </c>
-      <c r="E35" s="18">
+        <v>52.41</v>
+      </c>
+      <c r="D38" s="14">
         <f t="shared" si="3"/>
-        <v>54.188333333333333</v>
-      </c>
-      <c r="F35" s="18">
-        <f>ABS(D11-E11)</f>
-        <v>1.0499999999999972</v>
-      </c>
-      <c r="K35" s="18">
-        <f>B34</f>
-        <v>3</v>
-      </c>
-      <c r="L35" s="18">
-        <f>IF(C34 &gt;= $C$4 - $I$32,1,0)</f>
+        <v>0.4750655625000017</v>
+      </c>
+      <c r="E38" s="14">
+        <f t="shared" si="4"/>
+        <v>49.70333333333334</v>
+      </c>
+      <c r="F38" s="14">
+        <f t="shared" si="0"/>
+        <v>2.8200000000000003</v>
+      </c>
+      <c r="K38" s="14">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="L38" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M35" s="18">
+      <c r="M38" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="14">
+        <v>28</v>
+      </c>
+      <c r="Q38" s="14">
+        <v>1.7030000000000001</v>
+      </c>
+      <c r="R38" s="14">
+        <v>1.3140000000000001</v>
+      </c>
+      <c r="S38" s="14">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="2:19">
+      <c r="B39" s="14">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C39" s="14">
+        <f t="shared" si="2"/>
+        <v>49.15</v>
+      </c>
+      <c r="D39" s="14">
+        <f t="shared" si="3"/>
+        <v>15.596575562499995</v>
+      </c>
+      <c r="E39" s="14">
         <f t="shared" si="4"/>
+        <v>48.973333333333329</v>
+      </c>
+      <c r="F39" s="14">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="K39" s="14">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="L39" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="P35" s="18">
-        <v>25</v>
-      </c>
-      <c r="Q35" s="18">
-        <v>1.7110000000000001</v>
-      </c>
-      <c r="R35" s="18">
-        <v>1.3180000000000001</v>
-      </c>
-      <c r="S35" s="18">
-        <v>0.85699999999999998</v>
-      </c>
-    </row>
-    <row r="36" spans="2:19">
-      <c r="B36" s="18">
+      <c r="M39" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="14">
+        <v>29</v>
+      </c>
+      <c r="Q39" s="14">
+        <v>1.7010000000000001</v>
+      </c>
+      <c r="R39" s="14">
+        <v>1.3129999999999999</v>
+      </c>
+      <c r="S39" s="14">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="2:19">
+      <c r="B40" s="14">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C40" s="14">
+        <f t="shared" si="2"/>
+        <v>47.55</v>
+      </c>
+      <c r="D40" s="14">
+        <f t="shared" si="3"/>
+        <v>30.794175562500008</v>
+      </c>
+      <c r="E40" s="14">
+        <f t="shared" si="4"/>
+        <v>51.541666666666664</v>
+      </c>
+      <c r="F40" s="14">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="C36" s="18">
+        <v>3.8999999999999986</v>
+      </c>
+      <c r="K40" s="14">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="L40" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M40" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="14">
+        <v>30</v>
+      </c>
+      <c r="Q40" s="14">
+        <v>1.645</v>
+      </c>
+      <c r="R40" s="14">
+        <v>1.282</v>
+      </c>
+      <c r="S40" s="14">
+        <v>0.84199999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:19">
+      <c r="B41" s="14">
         <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C41" s="14">
+        <f t="shared" si="2"/>
+        <v>50.22</v>
+      </c>
+      <c r="D41" s="14">
+        <f t="shared" si="3"/>
+        <v>8.2900805624999947</v>
+      </c>
+      <c r="E41" s="14">
+        <f t="shared" si="4"/>
+        <v>53.096666666666671</v>
+      </c>
+      <c r="F41" s="14">
+        <f t="shared" si="0"/>
+        <v>4.68</v>
+      </c>
+      <c r="K41" s="14">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="L41" s="14">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="2:19">
+      <c r="B42" s="14">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="C42" s="14">
+        <f t="shared" si="2"/>
+        <v>56.855000000000004</v>
+      </c>
+      <c r="D42" s="14">
+        <f t="shared" si="3"/>
+        <v>14.105658062500046</v>
+      </c>
+      <c r="E42" s="14">
+        <f t="shared" si="4"/>
+        <v>54.535000000000004</v>
+      </c>
+      <c r="F42" s="14">
+        <f t="shared" si="0"/>
+        <v>0.50999999999999801</v>
+      </c>
+      <c r="K42" s="14">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="L42" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M42" s="14">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:19">
+      <c r="B43" s="14">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="C43" s="14">
+        <f t="shared" si="2"/>
+        <v>52.215000000000003</v>
+      </c>
+      <c r="D43" s="14">
+        <f t="shared" si="3"/>
+        <v>0.78189806249999017</v>
+      </c>
+      <c r="E43" s="14">
+        <f t="shared" si="4"/>
+        <v>53.633333333333333</v>
+      </c>
+      <c r="F43" s="14">
+        <f t="shared" si="0"/>
+        <v>0.27000000000000313</v>
+      </c>
+      <c r="K43" s="14">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="L43" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M43" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:19">
+      <c r="B44" s="14">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="C44" s="14">
+        <f t="shared" si="2"/>
+        <v>54.534999999999997</v>
+      </c>
+      <c r="D44" s="14">
+        <f t="shared" si="3"/>
+        <v>2.0613780624999962</v>
+      </c>
+      <c r="E44" s="14">
+        <f t="shared" si="4"/>
+        <v>55.076666666666675</v>
+      </c>
+      <c r="F44" s="14">
+        <f t="shared" si="0"/>
+        <v>1.4299999999999997</v>
+      </c>
+      <c r="K44" s="14">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="L44" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M44" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:19">
+      <c r="B45" s="14">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="C45" s="14">
+        <f t="shared" si="2"/>
         <v>54.15</v>
       </c>
-      <c r="D36" s="18">
+      <c r="D45" s="14">
+        <f t="shared" si="3"/>
+        <v>1.1040755625000016</v>
+      </c>
+      <c r="E45" s="14">
+        <f t="shared" si="4"/>
+        <v>56.023333333333333</v>
+      </c>
+      <c r="F45" s="14">
+        <f t="shared" si="0"/>
+        <v>0.65999999999999659</v>
+      </c>
+      <c r="K45" s="14">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="L45" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M45" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:19">
+      <c r="B46" s="14">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="C46" s="14">
         <f t="shared" si="2"/>
-        <v>1.1040755625000016</v>
-      </c>
-      <c r="E36" s="18">
+        <v>56.545000000000002</v>
+      </c>
+      <c r="D46" s="14">
         <f t="shared" si="3"/>
-        <v>53.416666666666664</v>
-      </c>
-      <c r="F36" s="18">
-        <f>ABS(D12-E12)</f>
-        <v>0.65999999999999659</v>
-      </c>
-      <c r="K36" s="18">
-        <f>B35</f>
-        <v>4</v>
-      </c>
-      <c r="L36" s="18">
-        <f>IF(C35 &gt;= $C$4 - $I$32,1,0)</f>
+        <v>11.873193062500027</v>
+      </c>
+      <c r="E46" s="14">
+        <f t="shared" si="4"/>
+        <v>56.37833333333333</v>
+      </c>
+      <c r="F46" s="14">
+        <f t="shared" si="0"/>
+        <v>2.490000000000002</v>
+      </c>
+      <c r="K46" s="14">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="L46" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M36" s="18">
-        <f t="shared" si="4"/>
+      <c r="M46" s="14">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P36" s="18">
-        <v>26</v>
-      </c>
-      <c r="Q36" s="18">
-        <v>1.708</v>
-      </c>
-      <c r="R36" s="18">
-        <v>1.3160000000000001</v>
-      </c>
-      <c r="S36" s="18">
-        <v>0.85599999999999998</v>
-      </c>
-    </row>
-    <row r="37" spans="2:19">
-      <c r="B37" s="18">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="C37" s="18">
-        <f t="shared" si="1"/>
-        <v>53.69</v>
-      </c>
-      <c r="D37" s="18">
-        <f t="shared" si="2"/>
-        <v>0.34898556249999985</v>
-      </c>
-      <c r="E37" s="18">
-        <f t="shared" si="3"/>
-        <v>51.75</v>
-      </c>
-      <c r="F37" s="18">
-        <f>ABS(D13-E13)</f>
-        <v>3.2199999999999989</v>
-      </c>
-      <c r="K37" s="18">
-        <f>B36</f>
-        <v>5</v>
-      </c>
-      <c r="L37" s="18">
-        <f>IF(C36 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M37" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P37" s="18">
-        <v>27</v>
-      </c>
-      <c r="Q37" s="18">
-        <v>1.706</v>
-      </c>
-      <c r="R37" s="18">
-        <v>1.3149999999999999</v>
-      </c>
-      <c r="S37" s="18">
-        <v>0.85599999999999998</v>
-      </c>
-    </row>
-    <row r="38" spans="2:19">
-      <c r="B38" s="18">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="C38" s="18">
-        <f t="shared" si="1"/>
-        <v>52.41</v>
-      </c>
-      <c r="D38" s="18">
-        <f t="shared" si="2"/>
-        <v>0.4750655625000017</v>
-      </c>
-      <c r="E38" s="18">
-        <f t="shared" si="3"/>
-        <v>49.70333333333334</v>
-      </c>
-      <c r="F38" s="18">
-        <f>ABS(D14-E14)</f>
-        <v>2.8200000000000003</v>
-      </c>
-      <c r="K38" s="18">
-        <f>B37</f>
-        <v>6</v>
-      </c>
-      <c r="L38" s="18">
-        <f>IF(C37 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M38" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P38" s="18">
-        <v>28</v>
-      </c>
-      <c r="Q38" s="18">
-        <v>1.7030000000000001</v>
-      </c>
-      <c r="R38" s="18">
-        <v>1.3140000000000001</v>
-      </c>
-      <c r="S38" s="18">
-        <v>0.85499999999999998</v>
-      </c>
-    </row>
-    <row r="39" spans="2:19">
-      <c r="B39" s="18">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="C39" s="18">
-        <f t="shared" si="1"/>
-        <v>49.15</v>
-      </c>
-      <c r="D39" s="18">
-        <f t="shared" si="2"/>
-        <v>15.596575562499995</v>
-      </c>
-      <c r="E39" s="18">
-        <f t="shared" si="3"/>
-        <v>48.973333333333329</v>
-      </c>
-      <c r="F39" s="18">
-        <f>ABS(D15-E15)</f>
-        <v>1.5</v>
-      </c>
-      <c r="K39" s="18">
-        <f>B38</f>
-        <v>7</v>
-      </c>
-      <c r="L39" s="18">
-        <f>IF(C38 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M39" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P39" s="18">
-        <v>29</v>
-      </c>
-      <c r="Q39" s="18">
-        <v>1.7010000000000001</v>
-      </c>
-      <c r="R39" s="18">
-        <v>1.3129999999999999</v>
-      </c>
-      <c r="S39" s="18">
-        <v>0.85499999999999998</v>
-      </c>
-    </row>
-    <row r="40" spans="2:19">
-      <c r="B40" s="18">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="C40" s="18">
-        <f t="shared" si="1"/>
-        <v>47.55</v>
-      </c>
-      <c r="D40" s="18">
-        <f t="shared" si="2"/>
-        <v>30.794175562500008</v>
-      </c>
-      <c r="E40" s="18">
-        <f t="shared" si="3"/>
-        <v>51.541666666666664</v>
-      </c>
-      <c r="F40" s="18">
-        <f>ABS(D16-E16)</f>
-        <v>3.8999999999999986</v>
-      </c>
-      <c r="K40" s="18">
-        <f>B39</f>
-        <v>8</v>
-      </c>
-      <c r="L40" s="18">
-        <f>IF(C39 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M40" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="P40" s="18">
-        <v>30</v>
-      </c>
-      <c r="Q40" s="18">
-        <v>1.645</v>
-      </c>
-      <c r="R40" s="18">
-        <v>1.282</v>
-      </c>
-      <c r="S40" s="18">
-        <v>0.84199999999999997</v>
-      </c>
-    </row>
-    <row r="41" spans="2:19">
-      <c r="B41" s="18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="C41" s="18">
-        <f t="shared" si="1"/>
-        <v>50.22</v>
-      </c>
-      <c r="D41" s="18">
-        <f t="shared" si="2"/>
-        <v>8.2900805624999947</v>
-      </c>
-      <c r="E41" s="18">
-        <f t="shared" si="3"/>
-        <v>53.096666666666671</v>
-      </c>
-      <c r="F41" s="18">
-        <f>ABS(D17-E17)</f>
-        <v>4.68</v>
-      </c>
-      <c r="K41" s="18">
-        <f>B40</f>
-        <v>9</v>
-      </c>
-      <c r="L41" s="18">
-        <f>IF(C40 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>0</v>
-      </c>
-      <c r="M41" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:19">
-      <c r="B42" s="18">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="C42" s="18">
-        <f t="shared" si="1"/>
-        <v>56.855000000000004</v>
-      </c>
-      <c r="D42" s="18">
-        <f t="shared" si="2"/>
-        <v>14.105658062500046</v>
-      </c>
-      <c r="E42" s="18">
-        <f t="shared" si="3"/>
-        <v>54.535000000000004</v>
-      </c>
-      <c r="F42" s="18">
-        <f>ABS(D18-E18)</f>
-        <v>0.50999999999999801</v>
-      </c>
-      <c r="K42" s="18">
-        <f>B41</f>
-        <v>10</v>
-      </c>
-      <c r="L42" s="18">
-        <f>IF(C41 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M42" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:19">
-      <c r="B43" s="18">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="C43" s="18">
-        <f t="shared" si="1"/>
-        <v>52.215000000000003</v>
-      </c>
-      <c r="D43" s="18">
-        <f t="shared" si="2"/>
-        <v>0.78189806249999017</v>
-      </c>
-      <c r="E43" s="18">
-        <f t="shared" si="3"/>
-        <v>53.633333333333333</v>
-      </c>
-      <c r="F43" s="18">
-        <f>ABS(D19-E19)</f>
-        <v>0.27000000000000313</v>
-      </c>
-      <c r="K43" s="18">
-        <f>B42</f>
-        <v>11</v>
-      </c>
-      <c r="L43" s="18">
-        <f>IF(C42 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M43" s="18">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="2:19">
-      <c r="B44" s="18">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="C44" s="18">
-        <f t="shared" si="1"/>
-        <v>54.534999999999997</v>
-      </c>
-      <c r="D44" s="18">
-        <f t="shared" si="2"/>
-        <v>2.0613780624999962</v>
-      </c>
-      <c r="E44" s="18">
-        <f t="shared" si="3"/>
-        <v>55.076666666666675</v>
-      </c>
-      <c r="F44" s="18">
-        <f>ABS(D20-E20)</f>
-        <v>1.4299999999999997</v>
-      </c>
-      <c r="K44" s="18">
-        <f>B43</f>
-        <v>12</v>
-      </c>
-      <c r="L44" s="18">
-        <f>IF(C43 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M44" s="18">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="2:19">
-      <c r="B45" s="18">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="C45" s="18">
-        <f t="shared" si="1"/>
-        <v>54.15</v>
-      </c>
-      <c r="D45" s="18">
-        <f t="shared" si="2"/>
-        <v>1.1040755625000016</v>
-      </c>
-      <c r="E45" s="18">
-        <f t="shared" si="3"/>
-        <v>56.023333333333333</v>
-      </c>
-      <c r="F45" s="18">
-        <f>ABS(D21-E21)</f>
-        <v>0.65999999999999659</v>
-      </c>
-      <c r="K45" s="18">
-        <f>B44</f>
-        <v>13</v>
-      </c>
-      <c r="L45" s="18">
-        <f>IF(C44 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M45" s="18">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="2:19">
-      <c r="B46" s="18">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="C46" s="18">
-        <f t="shared" si="1"/>
-        <v>56.545000000000002</v>
-      </c>
-      <c r="D46" s="18">
-        <f t="shared" si="2"/>
-        <v>11.873193062500027</v>
-      </c>
-      <c r="E46" s="18">
-        <f t="shared" si="3"/>
-        <v>56.37833333333333</v>
-      </c>
-      <c r="F46" s="18">
-        <f>ABS(D22-E22)</f>
-        <v>2.490000000000002</v>
-      </c>
-      <c r="K46" s="18">
-        <f>B45</f>
-        <v>14</v>
-      </c>
-      <c r="L46" s="18">
-        <f>IF(C45 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M46" s="18">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
     </row>
     <row r="47" spans="2:19">
-      <c r="B47" s="18">
+      <c r="B47" s="14">
         <f>B23</f>
         <v>16</v>
       </c>
-      <c r="C47" s="18">
+      <c r="C47" s="14">
+        <f t="shared" si="2"/>
+        <v>57.375</v>
+      </c>
+      <c r="D47" s="14">
+        <f t="shared" si="3"/>
+        <v>18.282038062500018</v>
+      </c>
+      <c r="E47" s="14">
+        <f t="shared" si="4"/>
+        <v>55.26</v>
+      </c>
+      <c r="F47" s="14">
+        <f t="shared" si="0"/>
+        <v>1.5499999999999972</v>
+      </c>
+      <c r="K47" s="14">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="L47" s="14">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="M47" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:19">
+      <c r="B48" s="14">
         <f t="shared" si="1"/>
-        <v>57.375</v>
-      </c>
-      <c r="D47" s="18">
+        <v>17</v>
+      </c>
+      <c r="C48" s="14">
         <f t="shared" si="2"/>
-        <v>18.282038062500018</v>
-      </c>
-      <c r="E47" s="18">
+        <v>55.215000000000003</v>
+      </c>
+      <c r="D48" s="14">
         <f t="shared" si="3"/>
-        <v>55.26</v>
-      </c>
-      <c r="F47" s="18">
-        <f>ABS(D23-E23)</f>
-        <v>1.5499999999999972</v>
-      </c>
-      <c r="K47" s="18">
-        <f>B46</f>
-        <v>15</v>
-      </c>
-      <c r="L47" s="18">
-        <f>IF(C46 &gt;= $C$4 - $I$32,1,0)</f>
+        <v>4.4763980625000235</v>
+      </c>
+      <c r="E48" s="14">
+        <f t="shared" si="4"/>
+        <v>51.814999999999998</v>
+      </c>
+      <c r="F48" s="14">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000284E-2</v>
+      </c>
+      <c r="K48" s="14">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="L48" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M47" s="18">
+      <c r="M48" s="14">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="2:13">
+      <c r="B49" s="14">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="C49" s="14">
+        <f t="shared" si="2"/>
+        <v>53.19</v>
+      </c>
+      <c r="D49" s="14">
+        <f t="shared" si="3"/>
+        <v>8.235562499999979E-3</v>
+      </c>
+      <c r="E49" s="14">
         <f t="shared" si="4"/>
+        <v>49.626666666666665</v>
+      </c>
+      <c r="F49" s="14">
+        <f t="shared" si="0"/>
+        <v>1.259999999999998</v>
+      </c>
+      <c r="K49" s="14">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="L49" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="2:19">
-      <c r="B48" s="18">
+      <c r="M49" s="14">
+        <f>IF(E48&gt;=$C$4+$I$31,1,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:13">
+      <c r="B50" s="14">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="C50" s="14">
+        <f t="shared" si="2"/>
+        <v>47.04</v>
+      </c>
+      <c r="D50" s="14">
+        <f t="shared" si="3"/>
+        <v>36.714510562499981</v>
+      </c>
+      <c r="F50" s="14">
         <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="C48" s="18">
-        <f t="shared" si="1"/>
-        <v>55.215000000000003</v>
-      </c>
-      <c r="D48" s="18">
-        <f t="shared" si="2"/>
-        <v>4.4763980625000235</v>
-      </c>
-      <c r="E48" s="18">
-        <f t="shared" si="3"/>
-        <v>51.814999999999998</v>
-      </c>
-      <c r="F48" s="18">
-        <f>ABS(D24-E24)</f>
-        <v>7.0000000000000284E-2</v>
-      </c>
-      <c r="K48" s="18">
-        <f>B47</f>
-        <v>16</v>
-      </c>
-      <c r="L48" s="18">
-        <f>IF(C47 &gt;= $C$4 - $I$32,1,0)</f>
+        <v>2.7199999999999989</v>
+      </c>
+      <c r="K50" s="14">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="L50" s="14">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M48" s="18">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="2:13">
-      <c r="B49" s="18">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="C49" s="18">
-        <f t="shared" si="1"/>
-        <v>53.19</v>
-      </c>
-      <c r="D49" s="18">
-        <f t="shared" si="2"/>
-        <v>8.235562499999979E-3</v>
-      </c>
-      <c r="E49" s="18">
-        <f t="shared" si="3"/>
-        <v>49.626666666666665</v>
-      </c>
-      <c r="F49" s="18">
-        <f>ABS(D25-E25)</f>
-        <v>1.259999999999998</v>
-      </c>
-      <c r="K49" s="18">
-        <f>B48</f>
-        <v>17</v>
-      </c>
-      <c r="L49" s="18">
-        <f>IF(C48 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M49" s="18">
-        <f t="shared" si="4"/>
+      <c r="M50" s="14">
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="2:13">
-      <c r="B50" s="18">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="C50" s="18">
-        <f t="shared" si="1"/>
-        <v>47.04</v>
-      </c>
-      <c r="D50" s="18">
-        <f t="shared" si="2"/>
-        <v>36.714510562499981</v>
-      </c>
-      <c r="F50" s="18">
-        <f>ABS(D26-E26)</f>
-        <v>2.7199999999999989</v>
-      </c>
-      <c r="K50" s="18">
-        <f>B49</f>
-        <v>18</v>
-      </c>
-      <c r="L50" s="18">
-        <f>IF(C49 &gt;= $C$4 - $I$32,1,0)</f>
-        <v>1</v>
-      </c>
-      <c r="M50" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="51" spans="2:13">
-      <c r="B51" s="18">
+      <c r="B51" s="14">
         <f>B27</f>
         <v>20</v>
       </c>
-      <c r="C51" s="18">
-        <f t="shared" si="1"/>
+      <c r="C51" s="14">
+        <f t="shared" si="2"/>
         <v>48.650000000000006</v>
       </c>
-      <c r="D51" s="18">
-        <f t="shared" si="2"/>
+      <c r="D51" s="14">
+        <f t="shared" si="3"/>
         <v>19.795825562499932</v>
       </c>
-      <c r="F51" s="18">
-        <f>ABS(D27-E27)</f>
+      <c r="F51" s="14">
+        <f t="shared" si="0"/>
         <v>1.8999999999999986</v>
       </c>
-      <c r="K51" s="18">
-        <f>B50</f>
+      <c r="K51" s="14">
+        <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="L51" s="18">
-        <f>IF(C50 &gt;= $C$4 - $I$32,1,0)</f>
+      <c r="L51" s="14">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M51" s="18">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
+      <c r="M51" s="14"/>
     </row>
     <row r="52" spans="2:13">
-      <c r="C52" s="31">
+      <c r="B52" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" s="23">
         <f>AVERAGE(C32:C51)</f>
         <v>53.099249999999998</v>
       </c>
-      <c r="D52" s="30">
+      <c r="D52" s="23">
         <f>SQRT((SUM(D32:D51)/(B51-1)))</f>
         <v>3.1065720975648428</v>
       </c>
-      <c r="K52" s="18">
-        <f>B51</f>
+      <c r="K52" s="14">
+        <f t="shared" si="5"/>
         <v>20</v>
       </c>
-      <c r="L52" s="18">
-        <f>IF(C51 &gt;= $C$4 - $I$32,1,0)</f>
+      <c r="L52" s="14">
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="M52" s="18">
-        <f t="shared" si="4"/>
+      <c r="M52" s="14"/>
+    </row>
+    <row r="54" spans="2:13">
+      <c r="D54" s="27"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="27"/>
+      <c r="K54" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="L54" s="28"/>
+    </row>
+    <row r="55" spans="2:13">
+      <c r="K55" s="28">
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:13">
-      <c r="D54" s="38"/>
-      <c r="E54" s="38"/>
-      <c r="F54" s="38"/>
-      <c r="K54" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="L54" s="39"/>
-    </row>
-    <row r="55" spans="2:13">
-      <c r="K55" s="39">
-        <v>0</v>
-      </c>
-      <c r="L55" s="39"/>
+      <c r="L55" s="28"/>
     </row>
     <row r="57" spans="2:13">
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="30" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="37"/>
+      <c r="C57" s="30"/>
+      <c r="K57" t="s">
+        <v>66</v>
+      </c>
+      <c r="L57">
+        <f>SUM(L33:L52)</f>
+        <v>16</v>
+      </c>
+      <c r="M57">
+        <f>SUM(M33:M52)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="58" spans="2:13">
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="C58" s="18">
+      <c r="C58" s="14">
         <f>AVERAGE(F32:F51)</f>
         <v>1.7914999999999992</v>
       </c>
+      <c r="K58" t="s">
+        <v>67</v>
+      </c>
+      <c r="L58">
+        <f>SUM(L57:M57)</f>
+        <v>26</v>
+      </c>
     </row>
     <row r="59" spans="2:13">
-      <c r="B59" s="32" t="s">
+      <c r="B59" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="C59" s="18">
+      <c r="C59" s="14">
         <v>1.1279999999999999</v>
       </c>
     </row>
     <row r="60" spans="2:13">
-      <c r="B60" s="32" t="s">
+      <c r="B60" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="C60" s="18">
+      <c r="C60" s="14">
         <f>C58/C59</f>
         <v>1.5882092198581554</v>
       </c>
     </row>
     <row r="61" spans="2:13">
-      <c r="B61" s="32" t="s">
+      <c r="B61" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="C61" s="35">
+      <c r="C61" s="25">
         <f>(C60/C52)*100</f>
         <v>2.9910200612214966</v>
       </c>
     </row>
     <row r="62" spans="2:13">
-      <c r="B62" s="39" t="str">
+      <c r="B62" s="28" t="str">
         <f>IF(C61&lt;=3,"Excelente",IF(C61&lt;=4,"Muy bueno",IF(C61&lt;=5,"Bueno",IF(C61&lt;=6,"Aceptable","Deficiente"))))</f>
         <v>Excelente</v>
       </c>
-      <c r="C62" s="39"/>
+      <c r="C62" s="28"/>
+    </row>
+    <row r="64" spans="2:13">
+      <c r="B64" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+    </row>
+    <row r="65" spans="2:8">
+      <c r="B65" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C65" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E65" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="F65" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="G65" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H65" s="24" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="66" spans="2:8">
+      <c r="B66" s="14">
+        <f>G8</f>
+        <v>1</v>
+      </c>
+      <c r="C66" s="14">
+        <f>K8/H8</f>
+        <v>1.2133333333333334</v>
+      </c>
+      <c r="D66" s="14">
+        <f>MAX(MIN(SLOPE($W$11:$W$16,$V$11:$V$16)*C66+(AVERAGE($W$11:$W$16)-SLOPE($W$11:$W$16,$V$11:$V$16)*AVERAGE($V$11:$V$16)),MAX($W$11:$W$16)),MIN($W$11:$W$16))</f>
+        <v>0.91245333333333345</v>
+      </c>
+      <c r="E66" s="14">
+        <f>(L8)*D66</f>
+        <v>47.630064000000012</v>
+      </c>
+      <c r="F66" s="14" cm="1">
+        <f t="array" ref="F66">IF(
+  L8&lt;MIN($V$19:$AC$19),
+  INDEX($V$20:$AC$20,1,1),
+  IF(
+    L8&gt;MAX($V$19:$AC$19),
+    INDEX($V$20:$AC$20,1,COLUMNS($V$20:$AC$20)),
+    IFERROR(
+      INDEX($V$20:$AC$20,1,MATCH(L8,$V$19:$AC$19,0)),
+      INDEX($V$20:$AC$20,1,MATCH(L8,$V$19:$AC$19,1)) +
+      (L8-INDEX($V$19:$AC$19,1,MATCH(L8,$V$19:$AC$19,1))) *
+      ( INDEX($V$20:$AC$20,1,MATCH(L8,$V$19:$AC$19,1)+1)
+       -INDEX($V$20:$AC$20,1,MATCH(L8,$V$19:$AC$19,1)) ) /
+      ( INDEX($V$19:$AC$19,1,MATCH(L8,$V$19:$AC$19,1)+1)
+       -INDEX($V$19:$AC$19,1,MATCH(L8,$V$19:$AC$19,1)) )
+    )
+  )
+)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G66" s="14">
+        <f>E66*F66</f>
+        <v>52.393070400000013</v>
+      </c>
+      <c r="H66" s="14">
+        <f>IF(E66&gt;=0.75*$C$4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="2:8">
+      <c r="B67" s="14">
+        <f t="shared" ref="B67:B68" si="8">G9</f>
+        <v>2</v>
+      </c>
+      <c r="C67" s="14">
+        <f t="shared" ref="C67:C68" si="9">K9/H9</f>
+        <v>1.2333333333333334</v>
+      </c>
+      <c r="D67" s="14">
+        <f t="shared" ref="D67:D68" si="10">MAX(MIN(SLOPE($W$11:$W$16,$V$11:$V$16)*C67+(AVERAGE($W$11:$W$16)-SLOPE($W$11:$W$16,$V$11:$V$16)*AVERAGE($V$11:$V$16)),MAX($W$11:$W$16)),MIN($W$11:$W$16))</f>
+        <v>0.91493333333333338</v>
+      </c>
+      <c r="E67" s="14">
+        <f t="shared" ref="E67:E68" si="11">(L9)*D67</f>
+        <v>48.948933333333336</v>
+      </c>
+      <c r="F67" s="14" cm="1">
+        <f t="array" ref="F67">IF(
+  L9&lt;MIN($V$19:$AC$19),
+  INDEX($V$20:$AC$20,1,1),
+  IF(
+    L9&gt;MAX($V$19:$AC$19),
+    INDEX($V$20:$AC$20,1,COLUMNS($V$20:$AC$20)),
+    IFERROR(
+      INDEX($V$20:$AC$20,1,MATCH(L9,$V$19:$AC$19,0)),
+      INDEX($V$20:$AC$20,1,MATCH(L9,$V$19:$AC$19,1)) +
+      (L9-INDEX($V$19:$AC$19,1,MATCH(L9,$V$19:$AC$19,1))) *
+      ( INDEX($V$20:$AC$20,1,MATCH(L9,$V$19:$AC$19,1)+1)
+       -INDEX($V$20:$AC$20,1,MATCH(L9,$V$19:$AC$19,1)) ) /
+      ( INDEX($V$19:$AC$19,1,MATCH(L9,$V$19:$AC$19,1)+1)
+       -INDEX($V$19:$AC$19,1,MATCH(L9,$V$19:$AC$19,1)) )
+    )
+  )
+)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G67" s="14">
+        <f t="shared" ref="G67:G68" si="12">E67*F67</f>
+        <v>53.843826666666672</v>
+      </c>
+      <c r="H67" s="14">
+        <f t="shared" ref="H67:H68" si="13">IF(E67&gt;=0.75*$C$4,1,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="2:8">
+      <c r="B68" s="14">
+        <f t="shared" si="8"/>
+        <v>3</v>
+      </c>
+      <c r="C68" s="14">
+        <f t="shared" si="9"/>
+        <v>1.2</v>
+      </c>
+      <c r="D68" s="14">
+        <f t="shared" si="10"/>
+        <v>0.91080000000000005</v>
+      </c>
+      <c r="E68" s="14">
+        <f t="shared" si="11"/>
+        <v>46.906200000000005</v>
+      </c>
+      <c r="F68" s="14" cm="1">
+        <f t="array" ref="F68">IF(
+  L10&lt;MIN($V$19:$AC$19),
+  INDEX($V$20:$AC$20,1,1),
+  IF(
+    L10&gt;MAX($V$19:$AC$19),
+    INDEX($V$20:$AC$20,1,COLUMNS($V$20:$AC$20)),
+    IFERROR(
+      INDEX($V$20:$AC$20,1,MATCH(L10,$V$19:$AC$19,0)),
+      INDEX($V$20:$AC$20,1,MATCH(L10,$V$19:$AC$19,1)) +
+      (L10-INDEX($V$19:$AC$19,1,MATCH(L10,$V$19:$AC$19,1))) *
+      ( INDEX($V$20:$AC$20,1,MATCH(L10,$V$19:$AC$19,1)+1)
+       -INDEX($V$20:$AC$20,1,MATCH(L10,$V$19:$AC$19,1)) ) /
+      ( INDEX($V$19:$AC$19,1,MATCH(L10,$V$19:$AC$19,1)+1)
+       -INDEX($V$19:$AC$19,1,MATCH(L10,$V$19:$AC$19,1)) )
+    )
+  )
+)</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G68" s="14">
+        <f t="shared" si="12"/>
+        <v>51.596820000000008</v>
+      </c>
+      <c r="H68" s="14">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="2:8">
+      <c r="B70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70">
+        <f>AVERAGE(E66:E68)</f>
+        <v>47.828399111111118</v>
+      </c>
+    </row>
+    <row r="71" spans="2:8">
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71">
+        <f>IF(C70&gt;=0.85*C4,1,0)</f>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="K54:L54"/>
-    <mergeCell ref="K55:L55"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="P10:S10"/>
-    <mergeCell ref="B57:C57"/>
+  <mergeCells count="15">
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="V18:AC18"/>
+    <mergeCell ref="B64:H64"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="K31:M31"/>
     <mergeCell ref="B29:N29"/>
@@ -2881,19 +3206,14 @@
     <mergeCell ref="P2:AB2"/>
     <mergeCell ref="P4:U4"/>
     <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="K55:L55"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="P10:S10"/>
+    <mergeCell ref="B57:C57"/>
   </mergeCells>
-  <conditionalFormatting sqref="L33:L52">
-    <cfRule type="colorScale" priority="8">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF2600"/>
-        <color theme="6" tint="0.39997558519241921"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="K55:L55">
-    <cfRule type="colorScale" priority="2">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2901,7 +3221,7 @@
         <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="5">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -2913,15 +3233,7 @@
         </ext>
       </extLst>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="colorScale" priority="5">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2937,9 +3249,7 @@
         <color rgb="FF00B050"/>
       </colorScale>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="L33:L52">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2948,7 +3258,45 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="L33:L52">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF2600"/>
+        <color theme="6" tint="0.39997558519241921"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="M33:M52">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C71">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66:H68">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3030,7 +3378,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="1"/>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="33" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3078,7 +3426,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="1"/>
-      <c r="B3" s="15"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="5">
         <v>65</v>
       </c>
@@ -3744,7 +4092,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="1"/>
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="35" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -3792,7 +4140,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="1"/>
-      <c r="B27" s="17"/>
+      <c r="B27" s="36"/>
       <c r="C27" s="11">
         <v>30</v>
       </c>
@@ -4458,7 +4806,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1"/>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -4506,7 +4854,7 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="1"/>
-      <c r="B51" s="15"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="5">
         <v>40</v>
       </c>
@@ -5172,7 +5520,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="1"/>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="35" t="s">
         <v>15</v>
       </c>
       <c r="C74" s="9" t="s">
@@ -5220,7 +5568,7 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="1"/>
-      <c r="B75" s="17"/>
+      <c r="B75" s="36"/>
       <c r="C75" s="11">
         <v>70</v>
       </c>
@@ -5886,7 +6234,7 @@
     </row>
     <row r="98" spans="1:18">
       <c r="A98" s="1"/>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="33" t="s">
         <v>16</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -5934,7 +6282,7 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="1"/>
-      <c r="B99" s="15"/>
+      <c r="B99" s="34"/>
       <c r="C99" s="5">
         <v>55</v>
       </c>
@@ -6600,7 +6948,7 @@
     </row>
     <row r="122" spans="1:18">
       <c r="A122" s="1"/>
-      <c r="B122" s="16" t="s">
+      <c r="B122" s="35" t="s">
         <v>17</v>
       </c>
       <c r="C122" s="9" t="s">
@@ -6648,7 +6996,7 @@
     </row>
     <row r="123" spans="1:18">
       <c r="A123" s="1"/>
-      <c r="B123" s="17"/>
+      <c r="B123" s="36"/>
       <c r="C123" s="11">
         <v>30</v>
       </c>
@@ -7314,7 +7662,7 @@
     </row>
     <row r="146" spans="1:18">
       <c r="A146" s="1"/>
-      <c r="B146" s="14" t="s">
+      <c r="B146" s="33" t="s">
         <v>18</v>
       </c>
       <c r="C146" s="3" t="s">
@@ -7362,7 +7710,7 @@
     </row>
     <row r="147" spans="1:18">
       <c r="A147" s="1"/>
-      <c r="B147" s="15"/>
+      <c r="B147" s="34"/>
       <c r="C147" s="5">
         <v>35</v>
       </c>
@@ -8028,7 +8376,7 @@
     </row>
     <row r="170" spans="1:18">
       <c r="A170" s="1"/>
-      <c r="B170" s="16" t="s">
+      <c r="B170" s="35" t="s">
         <v>19</v>
       </c>
       <c r="C170" s="9" t="s">
@@ -8076,7 +8424,7 @@
     </row>
     <row r="171" spans="1:18">
       <c r="A171" s="1"/>
-      <c r="B171" s="17"/>
+      <c r="B171" s="36"/>
       <c r="C171" s="11">
         <v>40</v>
       </c>
@@ -8742,7 +9090,7 @@
     </row>
     <row r="194" spans="1:18">
       <c r="A194" s="1"/>
-      <c r="B194" s="14" t="s">
+      <c r="B194" s="33" t="s">
         <v>20</v>
       </c>
       <c r="C194" s="3" t="s">
@@ -8790,7 +9138,7 @@
     </row>
     <row r="195" spans="1:18">
       <c r="A195" s="1"/>
-      <c r="B195" s="15"/>
+      <c r="B195" s="34"/>
       <c r="C195" s="5">
         <v>65</v>
       </c>
@@ -9456,7 +9804,7 @@
     </row>
     <row r="218" spans="1:18">
       <c r="A218" s="1"/>
-      <c r="B218" s="16" t="s">
+      <c r="B218" s="35" t="s">
         <v>21</v>
       </c>
       <c r="C218" s="9" t="s">
@@ -9504,7 +9852,7 @@
     </row>
     <row r="219" spans="1:18">
       <c r="A219" s="1"/>
-      <c r="B219" s="17"/>
+      <c r="B219" s="36"/>
       <c r="C219" s="11">
         <v>60</v>
       </c>
@@ -10170,7 +10518,7 @@
     </row>
     <row r="242" spans="1:18">
       <c r="A242" s="1"/>
-      <c r="B242" s="14" t="s">
+      <c r="B242" s="33" t="s">
         <v>22</v>
       </c>
       <c r="C242" s="3" t="s">
@@ -10218,7 +10566,7 @@
     </row>
     <row r="243" spans="1:18">
       <c r="A243" s="1"/>
-      <c r="B243" s="15"/>
+      <c r="B243" s="34"/>
       <c r="C243" s="5">
         <v>50</v>
       </c>
@@ -10884,7 +11232,7 @@
     </row>
     <row r="266" spans="1:18">
       <c r="A266" s="1"/>
-      <c r="B266" s="16" t="s">
+      <c r="B266" s="35" t="s">
         <v>23</v>
       </c>
       <c r="C266" s="9" t="s">
@@ -10932,7 +11280,7 @@
     </row>
     <row r="267" spans="1:18">
       <c r="A267" s="1"/>
-      <c r="B267" s="17"/>
+      <c r="B267" s="36"/>
       <c r="C267" s="11">
         <v>30</v>
       </c>
@@ -11598,7 +11946,7 @@
     </row>
     <row r="290" spans="1:18">
       <c r="A290" s="1"/>
-      <c r="B290" s="14" t="s">
+      <c r="B290" s="33" t="s">
         <v>24</v>
       </c>
       <c r="C290" s="3" t="s">
@@ -11646,7 +11994,7 @@
     </row>
     <row r="291" spans="1:18">
       <c r="A291" s="1"/>
-      <c r="B291" s="15"/>
+      <c r="B291" s="34"/>
       <c r="C291" s="5">
         <v>65</v>
       </c>
@@ -12312,7 +12660,7 @@
     </row>
     <row r="314" spans="1:18">
       <c r="A314" s="1"/>
-      <c r="B314" s="16" t="s">
+      <c r="B314" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C314" s="9" t="s">
@@ -12360,7 +12708,7 @@
     </row>
     <row r="315" spans="1:18">
       <c r="A315" s="1"/>
-      <c r="B315" s="17"/>
+      <c r="B315" s="36"/>
       <c r="C315" s="11">
         <v>40</v>
       </c>
@@ -13026,7 +13374,7 @@
     </row>
     <row r="338" spans="1:18">
       <c r="A338" s="1"/>
-      <c r="B338" s="14" t="s">
+      <c r="B338" s="33" t="s">
         <v>26</v>
       </c>
       <c r="C338" s="3" t="s">
@@ -13074,7 +13422,7 @@
     </row>
     <row r="339" spans="1:18">
       <c r="A339" s="1"/>
-      <c r="B339" s="15"/>
+      <c r="B339" s="34"/>
       <c r="C339" s="5">
         <v>70</v>
       </c>
@@ -13740,7 +14088,7 @@
     </row>
     <row r="362" spans="1:18">
       <c r="A362" s="1"/>
-      <c r="B362" s="16" t="s">
+      <c r="B362" s="35" t="s">
         <v>27</v>
       </c>
       <c r="C362" s="9" t="s">
@@ -13788,7 +14136,7 @@
     </row>
     <row r="363" spans="1:18">
       <c r="A363" s="1"/>
-      <c r="B363" s="17"/>
+      <c r="B363" s="36"/>
       <c r="C363" s="11">
         <v>55</v>
       </c>
@@ -14454,7 +14802,7 @@
     </row>
     <row r="386" spans="1:18">
       <c r="A386" s="1"/>
-      <c r="B386" s="14" t="s">
+      <c r="B386" s="33" t="s">
         <v>28</v>
       </c>
       <c r="C386" s="3" t="s">
@@ -14502,7 +14850,7 @@
     </row>
     <row r="387" spans="1:18">
       <c r="A387" s="1"/>
-      <c r="B387" s="15"/>
+      <c r="B387" s="34"/>
       <c r="C387" s="5">
         <v>30</v>
       </c>
@@ -15168,7 +15516,7 @@
     </row>
     <row r="410" spans="1:18">
       <c r="A410" s="1"/>
-      <c r="B410" s="16" t="s">
+      <c r="B410" s="35" t="s">
         <v>29</v>
       </c>
       <c r="C410" s="9" t="s">
@@ -15216,7 +15564,7 @@
     </row>
     <row r="411" spans="1:18">
       <c r="A411" s="1"/>
-      <c r="B411" s="17"/>
+      <c r="B411" s="36"/>
       <c r="C411" s="11">
         <v>35</v>
       </c>
@@ -24482,11 +24830,12 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B290:B291"/>
-    <mergeCell ref="B314:B315"/>
-    <mergeCell ref="B338:B339"/>
-    <mergeCell ref="B362:B363"/>
-    <mergeCell ref="B386:B387"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B98:B99"/>
     <mergeCell ref="B410:B411"/>
     <mergeCell ref="B146:B147"/>
     <mergeCell ref="B170:B171"/>
@@ -24494,12 +24843,11 @@
     <mergeCell ref="B218:B219"/>
     <mergeCell ref="B242:B243"/>
     <mergeCell ref="B266:B267"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="B290:B291"/>
+    <mergeCell ref="B314:B315"/>
+    <mergeCell ref="B338:B339"/>
+    <mergeCell ref="B362:B363"/>
+    <mergeCell ref="B386:B387"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
avance discusiones e intro
</commit_message>
<xml_diff>
--- a/Excel.xlsx
+++ b/Excel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukaswolff/Desktop/25_20/TECNOLOGIAS_DEL_HORMIGON/TAREAS/TALLER_HA_2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/db108f0a9d2e271a/Escritorio/202520/Tecnología del Hormigón/TALLER_HA_2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F9D201A-63E2-7045-ABCB-0F208C2C003A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{0F9D201A-63E2-7045-ABCB-0F208C2C003A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87BFE92E-67BE-4DA0-9CE6-E4BAA80C5F2E}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1020" windowWidth="38400" windowHeight="21600" xr2:uid="{9C17EDB2-E79E-E547-A673-26F1EAF70D3A}"/>
+    <workbookView xWindow="-28920" yWindow="4380" windowWidth="29040" windowHeight="15720" xr2:uid="{9C17EDB2-E79E-E547-A673-26F1EAF70D3A}"/>
   </bookViews>
   <sheets>
     <sheet name="DESARROLLO" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -353,6 +353,7 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -584,13 +585,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -599,16 +597,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -953,65 +954,68 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D97EA0-F291-AB40-8238-A1650B046FB5}">
   <dimension ref="B2:AC71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="119" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="61" workbookViewId="0">
+      <selection activeCell="S48" sqref="S48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.33203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.3125" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="5" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.1640625" customWidth="1"/>
-    <col min="7" max="8" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.8125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.4375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.8125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.1875" customWidth="1"/>
+    <col min="7" max="7" width="14.8125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.4375" customWidth="1"/>
+    <col min="9" max="9" width="14.8125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.9375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="19" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="18" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="4.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="5.1640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.8125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.6875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.8125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.0625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="7.4375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.0625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.1875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.9375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.3125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.0625" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="6.1875" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11.1875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="4.1875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:28">
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="P2" s="29" t="s">
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="P2" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="29"/>
-      <c r="R2" s="29"/>
-      <c r="S2" s="29"/>
-      <c r="T2" s="29"/>
-      <c r="U2" s="29"/>
-      <c r="V2" s="29"/>
-      <c r="W2" s="29"/>
-      <c r="X2" s="29"/>
-      <c r="Y2" s="29"/>
-      <c r="Z2" s="29"/>
-      <c r="AA2" s="29"/>
-      <c r="AB2" s="29"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
     </row>
     <row r="4" spans="2:28">
       <c r="B4" s="15" t="s">
@@ -1023,22 +1027,22 @@
       <c r="D4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="P4" s="30" t="s">
+      <c r="P4" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="W4" s="30" t="s">
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="W4" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="28"/>
+      <c r="AB4" s="28"/>
     </row>
     <row r="5" spans="2:28">
       <c r="B5" s="15" t="s">
@@ -1380,16 +1384,16 @@
         <f>DATOS!Q101</f>
         <v>45</v>
       </c>
-      <c r="P10" s="30" t="s">
+      <c r="P10" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="30"/>
-      <c r="S10" s="30"/>
-      <c r="V10" s="30" t="s">
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="V10" s="28" t="s">
         <v>69</v>
       </c>
-      <c r="W10" s="30"/>
+      <c r="W10" s="28"/>
     </row>
     <row r="11" spans="2:28">
       <c r="B11" s="14">
@@ -1416,11 +1420,11 @@
       <c r="L11" s="19"/>
       <c r="M11" s="19"/>
       <c r="P11" s="22"/>
-      <c r="Q11" s="29" t="s">
+      <c r="Q11" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
+      <c r="R11" s="32"/>
+      <c r="S11" s="32"/>
       <c r="V11" s="22" t="s">
         <v>70</v>
       </c>
@@ -1667,16 +1671,16 @@
       <c r="S18" s="14">
         <v>0.89600000000000002</v>
       </c>
-      <c r="V18" s="30" t="s">
+      <c r="V18" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="W18" s="30"/>
-      <c r="X18" s="30"/>
-      <c r="Y18" s="30"/>
-      <c r="Z18" s="30"/>
-      <c r="AA18" s="30"/>
-      <c r="AB18" s="30"/>
-      <c r="AC18" s="30"/>
+      <c r="W18" s="28"/>
+      <c r="X18" s="28"/>
+      <c r="Y18" s="28"/>
+      <c r="Z18" s="28"/>
+      <c r="AA18" s="28"/>
+      <c r="AB18" s="28"/>
+      <c r="AC18" s="28"/>
     </row>
     <row r="19" spans="2:29">
       <c r="B19" s="14">
@@ -2011,21 +2015,21 @@
       </c>
     </row>
     <row r="29" spans="2:29">
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31"/>
-      <c r="E29" s="31"/>
-      <c r="F29" s="31"/>
-      <c r="G29" s="31"/>
-      <c r="H29" s="31"/>
-      <c r="I29" s="31"/>
-      <c r="J29" s="31"/>
-      <c r="K29" s="31"/>
-      <c r="L29" s="31"/>
-      <c r="M29" s="31"/>
-      <c r="N29" s="31"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="F29" s="30"/>
+      <c r="G29" s="30"/>
+      <c r="H29" s="30"/>
+      <c r="I29" s="30"/>
+      <c r="J29" s="30"/>
+      <c r="K29" s="30"/>
+      <c r="L29" s="30"/>
+      <c r="M29" s="30"/>
+      <c r="N29" s="30"/>
       <c r="P29" s="14">
         <v>19</v>
       </c>
@@ -2086,11 +2090,11 @@
 )</f>
         <v>-1.5</v>
       </c>
-      <c r="K31" s="30" t="s">
+      <c r="K31" s="28" t="s">
         <v>51</v>
       </c>
-      <c r="L31" s="30"/>
-      <c r="M31" s="30"/>
+      <c r="L31" s="28"/>
+      <c r="M31" s="28"/>
       <c r="P31" s="14">
         <v>21</v>
       </c>
@@ -2927,22 +2931,22 @@
       <c r="D54" s="27"/>
       <c r="E54" s="27"/>
       <c r="F54" s="27"/>
-      <c r="K54" s="28" t="s">
+      <c r="K54" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="L54" s="28"/>
+      <c r="L54" s="29"/>
     </row>
     <row r="55" spans="2:13">
-      <c r="K55" s="28">
+      <c r="K55" s="29">
         <v>0</v>
       </c>
-      <c r="L55" s="28"/>
+      <c r="L55" s="29"/>
     </row>
     <row r="57" spans="2:13">
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="C57" s="30"/>
+      <c r="C57" s="28"/>
       <c r="K57" t="s">
         <v>66</v>
       </c>
@@ -2998,22 +3002,22 @@
       </c>
     </row>
     <row r="62" spans="2:13">
-      <c r="B62" s="28" t="str">
+      <c r="B62" s="29" t="str">
         <f>IF(C61&lt;=3,"Excelente",IF(C61&lt;=4,"Muy bueno",IF(C61&lt;=5,"Bueno",IF(C61&lt;=6,"Aceptable","Deficiente"))))</f>
         <v>Excelente</v>
       </c>
-      <c r="C62" s="28"/>
+      <c r="C62" s="29"/>
     </row>
     <row r="64" spans="2:13">
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="28" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="30"/>
-      <c r="D64" s="30"/>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
+      <c r="C64" s="28"/>
+      <c r="D64" s="28"/>
+      <c r="E64" s="28"/>
+      <c r="F64" s="28"/>
+      <c r="G64" s="28"/>
+      <c r="H64" s="28"/>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="24" t="s">
@@ -3196,22 +3200,42 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B2:N2"/>
+    <mergeCell ref="P2:AB2"/>
+    <mergeCell ref="P4:U4"/>
+    <mergeCell ref="W4:AB4"/>
+    <mergeCell ref="K54:L54"/>
+    <mergeCell ref="Q11:S11"/>
+    <mergeCell ref="P10:S10"/>
     <mergeCell ref="V10:W10"/>
     <mergeCell ref="V18:AC18"/>
     <mergeCell ref="B64:H64"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="K31:M31"/>
     <mergeCell ref="B29:N29"/>
-    <mergeCell ref="B2:N2"/>
-    <mergeCell ref="P2:AB2"/>
-    <mergeCell ref="P4:U4"/>
-    <mergeCell ref="W4:AB4"/>
-    <mergeCell ref="K54:L54"/>
     <mergeCell ref="K55:L55"/>
-    <mergeCell ref="Q11:S11"/>
-    <mergeCell ref="P10:S10"/>
     <mergeCell ref="B57:C57"/>
   </mergeCells>
+  <conditionalFormatting sqref="C71">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H66:H68">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="K55:L55">
     <cfRule type="colorScale" priority="4">
       <colorScale>
@@ -3286,26 +3310,6 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C71">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H66:H68">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FF00B050"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <extLst>
@@ -3336,24 +3340,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17C7A77D-5C2D-1348-8687-FC70E98F3FF7}">
   <dimension ref="A1:R863"/>
   <sheetViews>
-    <sheetView topLeftCell="A71" workbookViewId="0">
+    <sheetView topLeftCell="A52" zoomScale="44" workbookViewId="0">
       <selection activeCell="F98" sqref="F98:I98"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.8125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.6875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.3125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1875" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="11.8125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.8125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.6875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.3125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.3125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -3378,7 +3382,7 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="1"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="35" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -3426,7 +3430,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="1"/>
-      <c r="B3" s="34"/>
+      <c r="B3" s="36"/>
       <c r="C3" s="5">
         <v>65</v>
       </c>
@@ -4092,7 +4096,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="1"/>
-      <c r="B26" s="35" t="s">
+      <c r="B26" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="9" t="s">
@@ -4140,7 +4144,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" s="1"/>
-      <c r="B27" s="36"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="11">
         <v>30</v>
       </c>
@@ -4806,7 +4810,7 @@
     </row>
     <row r="50" spans="1:18">
       <c r="A50" s="1"/>
-      <c r="B50" s="33" t="s">
+      <c r="B50" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -4854,7 +4858,7 @@
     </row>
     <row r="51" spans="1:18">
       <c r="A51" s="1"/>
-      <c r="B51" s="34"/>
+      <c r="B51" s="36"/>
       <c r="C51" s="5">
         <v>40</v>
       </c>
@@ -5520,7 +5524,7 @@
     </row>
     <row r="74" spans="1:18">
       <c r="A74" s="1"/>
-      <c r="B74" s="35" t="s">
+      <c r="B74" s="33" t="s">
         <v>15</v>
       </c>
       <c r="C74" s="9" t="s">
@@ -5568,7 +5572,7 @@
     </row>
     <row r="75" spans="1:18">
       <c r="A75" s="1"/>
-      <c r="B75" s="36"/>
+      <c r="B75" s="34"/>
       <c r="C75" s="11">
         <v>70</v>
       </c>
@@ -6234,7 +6238,7 @@
     </row>
     <row r="98" spans="1:18">
       <c r="A98" s="1"/>
-      <c r="B98" s="33" t="s">
+      <c r="B98" s="35" t="s">
         <v>16</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -6282,7 +6286,7 @@
     </row>
     <row r="99" spans="1:18">
       <c r="A99" s="1"/>
-      <c r="B99" s="34"/>
+      <c r="B99" s="36"/>
       <c r="C99" s="5">
         <v>55</v>
       </c>
@@ -6948,7 +6952,7 @@
     </row>
     <row r="122" spans="1:18">
       <c r="A122" s="1"/>
-      <c r="B122" s="35" t="s">
+      <c r="B122" s="33" t="s">
         <v>17</v>
       </c>
       <c r="C122" s="9" t="s">
@@ -6996,7 +7000,7 @@
     </row>
     <row r="123" spans="1:18">
       <c r="A123" s="1"/>
-      <c r="B123" s="36"/>
+      <c r="B123" s="34"/>
       <c r="C123" s="11">
         <v>30</v>
       </c>
@@ -7662,7 +7666,7 @@
     </row>
     <row r="146" spans="1:18">
       <c r="A146" s="1"/>
-      <c r="B146" s="33" t="s">
+      <c r="B146" s="35" t="s">
         <v>18</v>
       </c>
       <c r="C146" s="3" t="s">
@@ -7710,7 +7714,7 @@
     </row>
     <row r="147" spans="1:18">
       <c r="A147" s="1"/>
-      <c r="B147" s="34"/>
+      <c r="B147" s="36"/>
       <c r="C147" s="5">
         <v>35</v>
       </c>
@@ -8376,7 +8380,7 @@
     </row>
     <row r="170" spans="1:18">
       <c r="A170" s="1"/>
-      <c r="B170" s="35" t="s">
+      <c r="B170" s="33" t="s">
         <v>19</v>
       </c>
       <c r="C170" s="9" t="s">
@@ -8424,7 +8428,7 @@
     </row>
     <row r="171" spans="1:18">
       <c r="A171" s="1"/>
-      <c r="B171" s="36"/>
+      <c r="B171" s="34"/>
       <c r="C171" s="11">
         <v>40</v>
       </c>
@@ -9090,7 +9094,7 @@
     </row>
     <row r="194" spans="1:18">
       <c r="A194" s="1"/>
-      <c r="B194" s="33" t="s">
+      <c r="B194" s="35" t="s">
         <v>20</v>
       </c>
       <c r="C194" s="3" t="s">
@@ -9138,7 +9142,7 @@
     </row>
     <row r="195" spans="1:18">
       <c r="A195" s="1"/>
-      <c r="B195" s="34"/>
+      <c r="B195" s="36"/>
       <c r="C195" s="5">
         <v>65</v>
       </c>
@@ -9804,7 +9808,7 @@
     </row>
     <row r="218" spans="1:18">
       <c r="A218" s="1"/>
-      <c r="B218" s="35" t="s">
+      <c r="B218" s="33" t="s">
         <v>21</v>
       </c>
       <c r="C218" s="9" t="s">
@@ -9852,7 +9856,7 @@
     </row>
     <row r="219" spans="1:18">
       <c r="A219" s="1"/>
-      <c r="B219" s="36"/>
+      <c r="B219" s="34"/>
       <c r="C219" s="11">
         <v>60</v>
       </c>
@@ -10518,7 +10522,7 @@
     </row>
     <row r="242" spans="1:18">
       <c r="A242" s="1"/>
-      <c r="B242" s="33" t="s">
+      <c r="B242" s="35" t="s">
         <v>22</v>
       </c>
       <c r="C242" s="3" t="s">
@@ -10566,7 +10570,7 @@
     </row>
     <row r="243" spans="1:18">
       <c r="A243" s="1"/>
-      <c r="B243" s="34"/>
+      <c r="B243" s="36"/>
       <c r="C243" s="5">
         <v>50</v>
       </c>
@@ -11232,7 +11236,7 @@
     </row>
     <row r="266" spans="1:18">
       <c r="A266" s="1"/>
-      <c r="B266" s="35" t="s">
+      <c r="B266" s="33" t="s">
         <v>23</v>
       </c>
       <c r="C266" s="9" t="s">
@@ -11280,7 +11284,7 @@
     </row>
     <row r="267" spans="1:18">
       <c r="A267" s="1"/>
-      <c r="B267" s="36"/>
+      <c r="B267" s="34"/>
       <c r="C267" s="11">
         <v>30</v>
       </c>
@@ -11946,7 +11950,7 @@
     </row>
     <row r="290" spans="1:18">
       <c r="A290" s="1"/>
-      <c r="B290" s="33" t="s">
+      <c r="B290" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C290" s="3" t="s">
@@ -11994,7 +11998,7 @@
     </row>
     <row r="291" spans="1:18">
       <c r="A291" s="1"/>
-      <c r="B291" s="34"/>
+      <c r="B291" s="36"/>
       <c r="C291" s="5">
         <v>65</v>
       </c>
@@ -12660,7 +12664,7 @@
     </row>
     <row r="314" spans="1:18">
       <c r="A314" s="1"/>
-      <c r="B314" s="35" t="s">
+      <c r="B314" s="33" t="s">
         <v>25</v>
       </c>
       <c r="C314" s="9" t="s">
@@ -12708,7 +12712,7 @@
     </row>
     <row r="315" spans="1:18">
       <c r="A315" s="1"/>
-      <c r="B315" s="36"/>
+      <c r="B315" s="34"/>
       <c r="C315" s="11">
         <v>40</v>
       </c>
@@ -13374,7 +13378,7 @@
     </row>
     <row r="338" spans="1:18">
       <c r="A338" s="1"/>
-      <c r="B338" s="33" t="s">
+      <c r="B338" s="35" t="s">
         <v>26</v>
       </c>
       <c r="C338" s="3" t="s">
@@ -13422,7 +13426,7 @@
     </row>
     <row r="339" spans="1:18">
       <c r="A339" s="1"/>
-      <c r="B339" s="34"/>
+      <c r="B339" s="36"/>
       <c r="C339" s="5">
         <v>70</v>
       </c>
@@ -14088,7 +14092,7 @@
     </row>
     <row r="362" spans="1:18">
       <c r="A362" s="1"/>
-      <c r="B362" s="35" t="s">
+      <c r="B362" s="33" t="s">
         <v>27</v>
       </c>
       <c r="C362" s="9" t="s">
@@ -14136,7 +14140,7 @@
     </row>
     <row r="363" spans="1:18">
       <c r="A363" s="1"/>
-      <c r="B363" s="36"/>
+      <c r="B363" s="34"/>
       <c r="C363" s="11">
         <v>55</v>
       </c>
@@ -14802,7 +14806,7 @@
     </row>
     <row r="386" spans="1:18">
       <c r="A386" s="1"/>
-      <c r="B386" s="33" t="s">
+      <c r="B386" s="35" t="s">
         <v>28</v>
       </c>
       <c r="C386" s="3" t="s">
@@ -14850,7 +14854,7 @@
     </row>
     <row r="387" spans="1:18">
       <c r="A387" s="1"/>
-      <c r="B387" s="34"/>
+      <c r="B387" s="36"/>
       <c r="C387" s="5">
         <v>30</v>
       </c>
@@ -15516,7 +15520,7 @@
     </row>
     <row r="410" spans="1:18">
       <c r="A410" s="1"/>
-      <c r="B410" s="35" t="s">
+      <c r="B410" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C410" s="9" t="s">
@@ -15564,7 +15568,7 @@
     </row>
     <row r="411" spans="1:18">
       <c r="A411" s="1"/>
-      <c r="B411" s="36"/>
+      <c r="B411" s="34"/>
       <c r="C411" s="11">
         <v>35</v>
       </c>
@@ -24830,12 +24834,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B50:B51"/>
-    <mergeCell ref="B74:B75"/>
-    <mergeCell ref="B98:B99"/>
     <mergeCell ref="B410:B411"/>
     <mergeCell ref="B146:B147"/>
     <mergeCell ref="B170:B171"/>
@@ -24848,6 +24846,12 @@
     <mergeCell ref="B338:B339"/>
     <mergeCell ref="B362:B363"/>
     <mergeCell ref="B386:B387"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="B74:B75"/>
+    <mergeCell ref="B98:B99"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>